<commit_message>
added data for metal track
</commit_message>
<xml_diff>
--- a/Semesteroppgave datasett.xlsx
+++ b/Semesteroppgave datasett.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sondreklyve/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sondreklyve/semesteroppgave/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B8C4D2-E93C-3A4F-9B81-4DE81B66975E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0106CEC5-E939-2F4F-A545-3BABF6943DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="3" xr2:uid="{0FBCAA18-910F-1F49-A720-95E14FF45760}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="4" xr2:uid="{0FBCAA18-910F-1F49-A720-95E14FF45760}"/>
   </bookViews>
   <sheets>
     <sheet name="Kule filt" sheetId="1" r:id="rId1"/>
     <sheet name="Sylinder filt" sheetId="2" r:id="rId2"/>
     <sheet name="Hul sylinder teip" sheetId="3" r:id="rId3"/>
     <sheet name="Sylinder teip" sheetId="4" r:id="rId4"/>
+    <sheet name="Sylinder metall" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="16">
   <si>
     <t>t</t>
   </si>
@@ -13266,11 +13267,11 @@
         <v>5.1929485136986198E-2</v>
       </c>
       <c r="D134" s="2">
-        <f t="shared" ref="D134:D140" si="9">(B134^2+C134^2)^0.5</f>
+        <f t="shared" ref="D134" si="9">(B134^2+C134^2)^0.5</f>
         <v>0.55365043275323433</v>
       </c>
       <c r="E134" s="2">
-        <f t="shared" ref="E134:E140" si="10">DEGREES(ATAN(B134/C134))</f>
+        <f t="shared" ref="E134" si="10">DEGREES(ATAN(B134/C134))</f>
         <v>84.618047628153022</v>
       </c>
     </row>
@@ -13379,8 +13380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DAD7AF0-2882-1740-B463-134761CADA88}">
   <dimension ref="A2:Q139"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+    <sheetView zoomScale="88" workbookViewId="0">
+      <selection activeCell="E23" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13546,11 +13547,11 @@
         <v>0.48206923363653298</v>
       </c>
       <c r="J6" s="4">
-        <f t="shared" ref="J6:J66" si="2">(H6^2+I6^2)^0.5</f>
+        <f t="shared" ref="J6:J55" si="2">(H6^2+I6^2)^0.5</f>
         <v>0.52106950915865613</v>
       </c>
       <c r="K6" s="2">
-        <f t="shared" ref="K6:K66" si="3">DEGREES(ATAN(H6/I6))</f>
+        <f t="shared" ref="K6:K55" si="3">DEGREES(ATAN(H6/I6))</f>
         <v>22.308500603626133</v>
       </c>
       <c r="M6" s="8">
@@ -16184,11 +16185,11 @@
         <v>0.51081474752840095</v>
       </c>
       <c r="D70" s="2">
-        <f t="shared" ref="D70:D133" si="7">(B70^2+C70^2)^0.5</f>
+        <f t="shared" ref="D70:D120" si="7">(B70^2+C70^2)^0.5</f>
         <v>0.52464182111522817</v>
       </c>
       <c r="E70" s="2">
-        <f t="shared" ref="E70:E133" si="8">DEGREES(ATAN(B70/C70))</f>
+        <f t="shared" ref="E70:E120" si="8">DEGREES(ATAN(B70/C70))</f>
         <v>13.183471515205724</v>
       </c>
       <c r="G70" s="1"/>
@@ -17277,5 +17278,3891 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B58BE6-65FB-F14F-AB37-8104F299DF65}">
+  <dimension ref="A3:Q139"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="11.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="2"/>
+    <col min="7" max="7" width="14.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.83203125" style="2"/>
+    <col min="13" max="13" width="16.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.83203125" style="2"/>
+    <col min="19" max="21" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M3" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" s="8">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2">
+        <v>6.8033508512901899E-3</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.52577190791052597</v>
+      </c>
+      <c r="D5" s="2">
+        <f>(B5^2+C5^2)^0.5</f>
+        <v>0.5258159228576863</v>
+      </c>
+      <c r="E5" s="2">
+        <f>DEGREES(ATAN(B5/C5))</f>
+        <v>0.74135101331604325</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.207054596183054</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0.479031140590161</v>
+      </c>
+      <c r="J5" s="4">
+        <f>(H5^2+I5^2)^0.5</f>
+        <v>0.52186438799331591</v>
+      </c>
+      <c r="K5" s="2">
+        <f>DEGREES(ATAN(H5/I5))</f>
+        <v>23.375747966941944</v>
+      </c>
+      <c r="M5" s="8">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2">
+        <v>0.35884431158658803</v>
+      </c>
+      <c r="O5" s="2">
+        <v>0.37839654112631899</v>
+      </c>
+      <c r="P5" s="2">
+        <f>(N5^2+O5^2)^0.5</f>
+        <v>0.52149130605832184</v>
+      </c>
+      <c r="Q5" s="2">
+        <f>DEGREES(ATAN(N5/O5))</f>
+        <v>43.480825237831169</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="B6" s="2">
+        <v>7.1056041920335902E-3</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.52577465993426498</v>
+      </c>
+      <c r="D6" s="2">
+        <f t="shared" ref="D6:D69" si="0">(B6^2+C6^2)^0.5</f>
+        <v>0.5258226722383943</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" ref="E6:E69" si="1">DEGREES(ATAN(B6/C6))</f>
+        <v>0.77427913307355167</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.20709147474748499</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.47948868611214901</v>
+      </c>
+      <c r="J6" s="4">
+        <f t="shared" ref="J6:J55" si="2">(H6^2+I6^2)^0.5</f>
+        <v>0.52229903218620188</v>
+      </c>
+      <c r="K6" s="2">
+        <f t="shared" ref="K6:K55" si="3">DEGREES(ATAN(H6/I6))</f>
+        <v>23.359547172456672</v>
+      </c>
+      <c r="M6" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="N6" s="2">
+        <v>0.35894166786591097</v>
+      </c>
+      <c r="O6" s="2">
+        <v>0.37838007221961401</v>
+      </c>
+      <c r="P6" s="2">
+        <f t="shared" ref="P6:P39" si="4">(N6^2+O6^2)^0.5</f>
+        <v>0.52154635458728138</v>
+      </c>
+      <c r="Q6" s="2">
+        <f t="shared" ref="Q6:Q35" si="5">DEGREES(ATAN(N6/O6))</f>
+        <v>43.48983076507232</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" s="8">
+        <v>1.9999999999999699E-2</v>
+      </c>
+      <c r="B7" s="2">
+        <v>7.3772567222858904E-3</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.52578065254603101</v>
+      </c>
+      <c r="D7" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52583240534268783</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="1"/>
+        <v>0.80386742587591165</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.20774266522302401</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0.47802060883319702</v>
+      </c>
+      <c r="J7" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52121081859764362</v>
+      </c>
+      <c r="K7" s="2">
+        <f t="shared" si="3"/>
+        <v>23.489252462939319</v>
+      </c>
+      <c r="M7" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="N7" s="2">
+        <v>0.35923800641626402</v>
+      </c>
+      <c r="O7" s="2">
+        <v>0.37825816954482699</v>
+      </c>
+      <c r="P7" s="2">
+        <f t="shared" si="4"/>
+        <v>0.5216619480864354</v>
+      </c>
+      <c r="Q7" s="2">
+        <f t="shared" si="5"/>
+        <v>43.522658707331246</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="8">
+        <v>2.9999999999999701E-2</v>
+      </c>
+      <c r="B8" s="2">
+        <v>6.8862574523167403E-3</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.52580742697211702</v>
+      </c>
+      <c r="D8" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52585251810820288</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="1"/>
+        <v>0.75033351164512485</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.20853581437016</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0.47710719766780502</v>
+      </c>
+      <c r="J8" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52069037243015337</v>
+      </c>
+      <c r="K8" s="2">
+        <f t="shared" si="3"/>
+        <v>23.609357976325246</v>
+      </c>
+      <c r="M8" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="N8" s="2">
+        <v>0.36080903341072001</v>
+      </c>
+      <c r="O8" s="2">
+        <v>0.381798369362705</v>
+      </c>
+      <c r="P8" s="2">
+        <f t="shared" si="4"/>
+        <v>0.52531243411782913</v>
+      </c>
+      <c r="Q8" s="2">
+        <f t="shared" si="5"/>
+        <v>43.381001493811944</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" s="8">
+        <v>3.9999999999999702E-2</v>
+      </c>
+      <c r="B9" s="2">
+        <v>6.6689700093117699E-3</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.52578739467430102</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52582968683726317</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="1"/>
+        <v>0.72668791674240629</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.20921918775954401</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0.47585324125908202</v>
+      </c>
+      <c r="J9" s="4">
+        <f t="shared" si="2"/>
+        <v>0.51981629037914678</v>
+      </c>
+      <c r="K9" s="2">
+        <f t="shared" si="3"/>
+        <v>23.733731774553689</v>
+      </c>
+      <c r="M9" s="8">
+        <v>0.04</v>
+      </c>
+      <c r="N9" s="2">
+        <v>0.35993427208334999</v>
+      </c>
+      <c r="O9" s="2">
+        <v>0.38197383113118799</v>
+      </c>
+      <c r="P9" s="2">
+        <f t="shared" si="4"/>
+        <v>0.52483967827252576</v>
+      </c>
+      <c r="Q9" s="2">
+        <f t="shared" si="5"/>
+        <v>43.298438244921009</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" s="8">
+        <v>4.9999999999999697E-2</v>
+      </c>
+      <c r="B10" s="2">
+        <v>6.5571730402412803E-3</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.52580694033430297</v>
+      </c>
+      <c r="D10" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52584782496650195</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="1"/>
+        <v>0.71448061596450696</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.21019225794632701</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0.47449962477957403</v>
+      </c>
+      <c r="J10" s="4">
+        <f t="shared" si="2"/>
+        <v>0.51897078840386746</v>
+      </c>
+      <c r="K10" s="2">
+        <f t="shared" si="3"/>
+        <v>23.892224588805352</v>
+      </c>
+      <c r="M10" s="8">
+        <v>5.00000000000001E-2</v>
+      </c>
+      <c r="N10" s="2">
+        <v>0.36044787493292701</v>
+      </c>
+      <c r="O10" s="2">
+        <v>0.381964866160101</v>
+      </c>
+      <c r="P10" s="2">
+        <f t="shared" si="4"/>
+        <v>0.52518551914953526</v>
+      </c>
+      <c r="Q10" s="2">
+        <f t="shared" si="5"/>
+        <v>43.339888712577093</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" s="8">
+        <v>5.9999999999999699E-2</v>
+      </c>
+      <c r="B11" s="2">
+        <v>8.1732210017364491E-3</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.52574799673810602</v>
+      </c>
+      <c r="D11" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52581152290119582</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="1"/>
+        <v>0.89064219378251264</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.21151830097077601</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0.47280820705597998</v>
+      </c>
+      <c r="J11" s="4">
+        <f t="shared" si="2"/>
+        <v>0.51796485624514543</v>
+      </c>
+      <c r="K11" s="2">
+        <f t="shared" si="3"/>
+        <v>24.102117363968421</v>
+      </c>
+      <c r="M11" s="8">
+        <v>6.0000000000000102E-2</v>
+      </c>
+      <c r="N11" s="2">
+        <v>0.36348701062601402</v>
+      </c>
+      <c r="O11" s="2">
+        <v>0.38216172117179698</v>
+      </c>
+      <c r="P11" s="2">
+        <f t="shared" si="4"/>
+        <v>0.52741860796034334</v>
+      </c>
+      <c r="Q11" s="2">
+        <f t="shared" si="5"/>
+        <v>43.565331875750957</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" s="8">
+        <v>6.9999999999999701E-2</v>
+      </c>
+      <c r="B12" s="2">
+        <v>8.4555372824908197E-3</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.52576963378489505</v>
+      </c>
+      <c r="D12" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52583762124922007</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="1"/>
+        <v>0.92136328932842282</v>
+      </c>
+      <c r="G12" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0.21302426923884399</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0.47090141796268098</v>
+      </c>
+      <c r="J12" s="4">
+        <f t="shared" si="2"/>
+        <v>0.51684377206657628</v>
+      </c>
+      <c r="K12" s="2">
+        <f t="shared" si="3"/>
+        <v>24.340831097301031</v>
+      </c>
+      <c r="M12" s="8">
+        <v>7.0000000000000104E-2</v>
+      </c>
+      <c r="N12" s="2">
+        <v>0.36553088486597102</v>
+      </c>
+      <c r="O12" s="2">
+        <v>0.37883553471637899</v>
+      </c>
+      <c r="P12" s="2">
+        <f t="shared" si="4"/>
+        <v>0.52643061285866022</v>
+      </c>
+      <c r="Q12" s="2">
+        <f t="shared" si="5"/>
+        <v>43.976016244333628</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" s="8">
+        <v>7.9999999999999696E-2</v>
+      </c>
+      <c r="B13" s="2">
+        <v>8.5736269219103805E-3</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.52577784607302303</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52584774459893202</v>
+      </c>
+      <c r="E13" s="2">
+        <f t="shared" si="1"/>
+        <v>0.93421415174744205</v>
+      </c>
+      <c r="G13" s="1">
+        <v>8.0000000000000196E-2</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0.213201996314836</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0.47789596821517299</v>
+      </c>
+      <c r="J13" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52329690202498713</v>
+      </c>
+      <c r="K13" s="2">
+        <f t="shared" si="3"/>
+        <v>24.04291060810667</v>
+      </c>
+      <c r="M13" s="8">
+        <v>8.0000000000000099E-2</v>
+      </c>
+      <c r="N13" s="2">
+        <v>0.36752565420246602</v>
+      </c>
+      <c r="O13" s="2">
+        <v>0.37472519881416599</v>
+      </c>
+      <c r="P13" s="2">
+        <f t="shared" si="4"/>
+        <v>0.52487530054601239</v>
+      </c>
+      <c r="Q13" s="2">
+        <f t="shared" si="5"/>
+        <v>44.444270648834824</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" s="8">
+        <v>8.9999999999999705E-2</v>
+      </c>
+      <c r="B14" s="2">
+        <v>9.1708307426402406E-3</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.52573057898167397</v>
+      </c>
+      <c r="D14" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52581056076586774</v>
+      </c>
+      <c r="E14" s="2">
+        <f t="shared" si="1"/>
+        <v>0.99936475095810495</v>
+      </c>
+      <c r="G14" s="1">
+        <v>9.0000000000000205E-2</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0.217441189745914</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0.48077367506906499</v>
+      </c>
+      <c r="J14" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52765897854346555</v>
+      </c>
+      <c r="K14" s="2">
+        <f t="shared" si="3"/>
+        <v>24.335978759423941</v>
+      </c>
+      <c r="M14" s="8">
+        <v>9.0000000000000094E-2</v>
+      </c>
+      <c r="N14" s="2">
+        <v>0.36954928668793602</v>
+      </c>
+      <c r="O14" s="2">
+        <v>0.37358585108730002</v>
+      </c>
+      <c r="P14" s="2">
+        <f t="shared" si="4"/>
+        <v>0.52548364715201623</v>
+      </c>
+      <c r="Q14" s="2">
+        <f t="shared" si="5"/>
+        <v>44.688783617515675</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" s="8">
+        <v>9.99999999999997E-2</v>
+      </c>
+      <c r="B15" s="2">
+        <v>9.7961421134194395E-3</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.52568348564740397</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="0"/>
+        <v>0.5257747535615519</v>
+      </c>
+      <c r="E15" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0675865928963186</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0.218826650402241</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0.47625598585305501</v>
+      </c>
+      <c r="J15" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52412295025798095</v>
+      </c>
+      <c r="K15" s="2">
+        <f t="shared" si="3"/>
+        <v>24.677492212063949</v>
+      </c>
+      <c r="M15" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="N15" s="2">
+        <v>0.373659575087394</v>
+      </c>
+      <c r="O15" s="2">
+        <v>0.37034277317704201</v>
+      </c>
+      <c r="P15" s="2">
+        <f t="shared" si="4"/>
+        <v>0.52609433346022061</v>
+      </c>
+      <c r="Q15" s="2">
+        <f t="shared" si="5"/>
+        <v>45.255425930367089</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16" s="8">
+        <v>0.109999999999999</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1.04633374746181E-2</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.52574485715829899</v>
+      </c>
+      <c r="D16" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52584896715645257</v>
+      </c>
+      <c r="E16" s="2">
+        <f t="shared" si="1"/>
+        <v>1.1401460909016439</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0.22508538271741799</v>
+      </c>
+      <c r="I16" s="2">
+        <v>0.47809658680952699</v>
+      </c>
+      <c r="J16" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52843142964056</v>
+      </c>
+      <c r="K16" s="2">
+        <f t="shared" si="3"/>
+        <v>25.210811969020757</v>
+      </c>
+      <c r="M16" s="8">
+        <v>0.11</v>
+      </c>
+      <c r="N16" s="2">
+        <v>0.37611854407940298</v>
+      </c>
+      <c r="O16" s="2">
+        <v>0.36730607226824302</v>
+      </c>
+      <c r="P16" s="2">
+        <f t="shared" si="4"/>
+        <v>0.52571751913507081</v>
+      </c>
+      <c r="Q16" s="2">
+        <f t="shared" si="5"/>
+        <v>45.679145919190873</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A17" s="8">
+        <v>0.119999999999999</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1.1047125950934201E-2</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.52568564313890798</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" si="0"/>
+        <v>0.5258017063438869</v>
+      </c>
+      <c r="E17" s="2">
+        <f t="shared" si="1"/>
+        <v>1.2038764063286909</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0.222396192426637</v>
+      </c>
+      <c r="I17" s="2">
+        <v>0.47465187560543298</v>
+      </c>
+      <c r="J17" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52417026758642193</v>
+      </c>
+      <c r="K17" s="2">
+        <f t="shared" si="3"/>
+        <v>25.105246899420841</v>
+      </c>
+      <c r="M17" s="8">
+        <v>0.12</v>
+      </c>
+      <c r="N17" s="2">
+        <v>0.38310829219824799</v>
+      </c>
+      <c r="O17" s="2">
+        <v>0.364198846361874</v>
+      </c>
+      <c r="P17" s="2">
+        <f t="shared" si="4"/>
+        <v>0.52859508439104697</v>
+      </c>
+      <c r="Q17" s="2">
+        <f t="shared" si="5"/>
+        <v>46.449471368238633</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A18" s="8">
+        <v>0.12999999999999901</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1.5361778637138499E-2</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.52461135920550195</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52483622440751998</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="shared" si="1"/>
+        <v>1.6772676200366037</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0.13</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0.22537998389073599</v>
+      </c>
+      <c r="I18" s="2">
+        <v>0.47259988051252799</v>
+      </c>
+      <c r="J18" s="4">
+        <f t="shared" si="2"/>
+        <v>0.5235902827584219</v>
+      </c>
+      <c r="K18" s="2">
+        <f t="shared" si="3"/>
+        <v>25.496187936413765</v>
+      </c>
+      <c r="M18" s="8">
+        <v>0.13</v>
+      </c>
+      <c r="N18" s="2">
+        <v>0.38844443341372997</v>
+      </c>
+      <c r="O18" s="2">
+        <v>0.358851874101211</v>
+      </c>
+      <c r="P18" s="2">
+        <f t="shared" si="4"/>
+        <v>0.5288324360287151</v>
+      </c>
+      <c r="Q18" s="2">
+        <f t="shared" si="5"/>
+        <v>47.267699311671407</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A19" s="8">
+        <v>0.13999999999999899</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1.23429122962161E-2</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.52570135923918704</v>
+      </c>
+      <c r="D19" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52584623854305634</v>
+      </c>
+      <c r="E19" s="2">
+        <f t="shared" si="1"/>
+        <v>1.3449972347690997</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0.231563484452567</v>
+      </c>
+      <c r="I19" s="2">
+        <v>0.46986644894843499</v>
+      </c>
+      <c r="J19" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52382833751070257</v>
+      </c>
+      <c r="K19" s="2">
+        <f t="shared" si="3"/>
+        <v>26.235382694233003</v>
+      </c>
+      <c r="M19" s="8">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="N19" s="2">
+        <v>0.39176231831261998</v>
+      </c>
+      <c r="O19" s="2">
+        <v>0.35110646982765198</v>
+      </c>
+      <c r="P19" s="2">
+        <f t="shared" si="4"/>
+        <v>0.52607363287330267</v>
+      </c>
+      <c r="Q19" s="2">
+        <f t="shared" si="5"/>
+        <v>48.132568063560313</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A20" s="8">
+        <v>0.149999999999999</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1.87645670574366E-2</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.52361664709237499</v>
+      </c>
+      <c r="D20" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52395276704023031</v>
+      </c>
+      <c r="E20" s="2">
+        <f t="shared" si="1"/>
+        <v>2.0523996151581199</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="H20" s="2">
+        <v>0.23616955053709099</v>
+      </c>
+      <c r="I20" s="2">
+        <v>0.46875818065931801</v>
+      </c>
+      <c r="J20" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52489073961723254</v>
+      </c>
+      <c r="K20" s="2">
+        <f t="shared" si="3"/>
+        <v>26.739860287294846</v>
+      </c>
+      <c r="M20" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="N20" s="2">
+        <v>0.39775031878205303</v>
+      </c>
+      <c r="O20" s="2">
+        <v>0.34487983804167899</v>
+      </c>
+      <c r="P20" s="2">
+        <f t="shared" si="4"/>
+        <v>0.52644792598972168</v>
+      </c>
+      <c r="Q20" s="2">
+        <f t="shared" si="5"/>
+        <v>49.072219446157703</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A21" s="8">
+        <v>0.159999999999999</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1.1129528466238801E-2</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.52667617280925705</v>
+      </c>
+      <c r="D21" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52679375224929081</v>
+      </c>
+      <c r="E21" s="2">
+        <f t="shared" si="1"/>
+        <v>1.2105733092819841</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0.16</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0.240784584650239</v>
+      </c>
+      <c r="I21" s="2">
+        <v>0.46816369038595201</v>
+      </c>
+      <c r="J21" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52645461076999001</v>
+      </c>
+      <c r="K21" s="2">
+        <f t="shared" si="3"/>
+        <v>27.21753300003499</v>
+      </c>
+      <c r="M21" s="15">
+        <v>0.16</v>
+      </c>
+      <c r="N21" s="13">
+        <v>0.40387362739639998</v>
+      </c>
+      <c r="O21" s="13">
+        <v>0.33856484213171001</v>
+      </c>
+      <c r="P21" s="13">
+        <f t="shared" si="4"/>
+        <v>0.52701049252742194</v>
+      </c>
+      <c r="Q21" s="2">
+        <f t="shared" si="5"/>
+        <v>50.027097823219385</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A22" s="8">
+        <v>0.16999999999999901</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1.93219241253073E-2</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.52346996782863797</v>
+      </c>
+      <c r="D22" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52382644451232074</v>
+      </c>
+      <c r="E22" s="2">
+        <f t="shared" si="1"/>
+        <v>2.1138984345255185</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0.17</v>
+      </c>
+      <c r="H22" s="2">
+        <v>0.244345158646011</v>
+      </c>
+      <c r="I22" s="2">
+        <v>0.46604580212257701</v>
+      </c>
+      <c r="J22" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52621596918928681</v>
+      </c>
+      <c r="K22" s="2">
+        <f t="shared" si="3"/>
+        <v>27.667766589732224</v>
+      </c>
+      <c r="M22" s="8">
+        <v>0.17</v>
+      </c>
+      <c r="N22" s="2">
+        <v>0.41143423060267598</v>
+      </c>
+      <c r="O22" s="2">
+        <v>0.330212721972169</v>
+      </c>
+      <c r="P22" s="2">
+        <f t="shared" si="4"/>
+        <v>0.52755906575840861</v>
+      </c>
+      <c r="Q22" s="2">
+        <f t="shared" si="5"/>
+        <v>51.249844065218198</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A23" s="8">
+        <v>0.17999999999999899</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1.53854991873093E-2</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.52564441716834798</v>
+      </c>
+      <c r="D23" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52586953409138937</v>
+      </c>
+      <c r="E23" s="2">
+        <f t="shared" si="1"/>
+        <v>1.676556489107647</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0.18</v>
+      </c>
+      <c r="H23" s="2">
+        <v>0.24404088753296799</v>
+      </c>
+      <c r="I23" s="2">
+        <v>0.46692468334258003</v>
+      </c>
+      <c r="J23" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52685350402407627</v>
+      </c>
+      <c r="K23" s="2">
+        <f t="shared" si="3"/>
+        <v>27.594078897464822</v>
+      </c>
+      <c r="M23" s="8">
+        <v>0.18</v>
+      </c>
+      <c r="N23" s="2">
+        <v>0.41847226598828702</v>
+      </c>
+      <c r="O23" s="2">
+        <v>0.32135596393413701</v>
+      </c>
+      <c r="P23" s="2">
+        <f t="shared" si="4"/>
+        <v>0.52762552341353808</v>
+      </c>
+      <c r="Q23" s="2">
+        <f t="shared" si="5"/>
+        <v>52.478384511053839</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A24" s="8">
+        <v>0.189999999999999</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1.0265961286320799E-2</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.52877925474929399</v>
+      </c>
+      <c r="D24" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52887889938468047</v>
+      </c>
+      <c r="E24" s="2">
+        <f t="shared" si="1"/>
+        <v>1.1122266325461438</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0.19</v>
+      </c>
+      <c r="H24" s="2">
+        <v>0.256559246651961</v>
+      </c>
+      <c r="I24" s="2">
+        <v>0.45915145523082901</v>
+      </c>
+      <c r="J24" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52596835064784053</v>
+      </c>
+      <c r="K24" s="2">
+        <f t="shared" si="3"/>
+        <v>29.195071622463892</v>
+      </c>
+      <c r="M24" s="8">
+        <v>0.19</v>
+      </c>
+      <c r="N24" s="2">
+        <v>0.42768369187680499</v>
+      </c>
+      <c r="O24" s="2">
+        <v>0.31099412166982898</v>
+      </c>
+      <c r="P24" s="2">
+        <f t="shared" si="4"/>
+        <v>0.52880117625678769</v>
+      </c>
+      <c r="Q24" s="2">
+        <f t="shared" si="5"/>
+        <v>53.976882065104242</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A25" s="8">
+        <v>0.19999999999999901</v>
+      </c>
+      <c r="B25" s="2">
+        <v>1.15472833287331E-2</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.52898033219131002</v>
+      </c>
+      <c r="D25" s="2">
+        <f t="shared" si="0"/>
+        <v>0.5291063518778647</v>
+      </c>
+      <c r="E25" s="2">
+        <f t="shared" si="1"/>
+        <v>1.2505295551858779</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0.263148680570506</v>
+      </c>
+      <c r="I25" s="2">
+        <v>0.45389709070119699</v>
+      </c>
+      <c r="J25" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52466160240006976</v>
+      </c>
+      <c r="K25" s="2">
+        <f t="shared" si="3"/>
+        <v>30.103187728916001</v>
+      </c>
+      <c r="M25" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="N25" s="2">
+        <v>0.43252144184625102</v>
+      </c>
+      <c r="O25" s="2">
+        <v>0.30210163930934097</v>
+      </c>
+      <c r="P25" s="2">
+        <f t="shared" si="4"/>
+        <v>0.52757956568668496</v>
+      </c>
+      <c r="Q25" s="2">
+        <f t="shared" si="5"/>
+        <v>55.06699955953799</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A26" s="8">
+        <v>0.21</v>
+      </c>
+      <c r="B26" s="2">
+        <v>1.1245361197293E-2</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.529676554989155</v>
+      </c>
+      <c r="D26" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52979591453090402</v>
+      </c>
+      <c r="E26" s="2">
+        <f t="shared" si="1"/>
+        <v>1.2162421581487515</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0.26926917661641597</v>
+      </c>
+      <c r="I26" s="2">
+        <v>0.45122058427895201</v>
+      </c>
+      <c r="J26" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52545780530193054</v>
+      </c>
+      <c r="K26" s="2">
+        <f t="shared" si="3"/>
+        <v>30.826948465886055</v>
+      </c>
+      <c r="M26" s="8">
+        <v>0.21</v>
+      </c>
+      <c r="N26" s="2">
+        <v>0.44264967400016603</v>
+      </c>
+      <c r="O26" s="2">
+        <v>0.28868783681471499</v>
+      </c>
+      <c r="P26" s="2">
+        <f t="shared" si="4"/>
+        <v>0.52846892152444758</v>
+      </c>
+      <c r="Q26" s="2">
+        <f t="shared" si="5"/>
+        <v>56.888361372223464</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A27" s="8">
+        <v>0.22</v>
+      </c>
+      <c r="B27" s="2">
+        <v>1.25171509993203E-2</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.52988913057889198</v>
+      </c>
+      <c r="D27" s="2">
+        <f t="shared" si="0"/>
+        <v>0.53003695132961615</v>
+      </c>
+      <c r="E27" s="2">
+        <f t="shared" si="1"/>
+        <v>1.3532011311637464</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0.22</v>
+      </c>
+      <c r="H27" s="2">
+        <v>0.27639929263658403</v>
+      </c>
+      <c r="I27" s="2">
+        <v>0.44749858576795398</v>
+      </c>
+      <c r="J27" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52597676111623304</v>
+      </c>
+      <c r="K27" s="2">
+        <f t="shared" si="3"/>
+        <v>31.701717652618985</v>
+      </c>
+      <c r="M27" s="15">
+        <v>0.22</v>
+      </c>
+      <c r="N27" s="13">
+        <v>0.44856227430491802</v>
+      </c>
+      <c r="O27" s="13">
+        <v>0.279216234853155</v>
+      </c>
+      <c r="P27" s="13">
+        <f t="shared" si="4"/>
+        <v>0.52836523327635099</v>
+      </c>
+      <c r="Q27" s="13">
+        <f t="shared" si="5"/>
+        <v>58.099004863434295</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A28" s="8">
+        <v>0.23</v>
+      </c>
+      <c r="B28" s="2">
+        <v>1.26535163144917E-2</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0.53078247440797499</v>
+      </c>
+      <c r="D28" s="2">
+        <f t="shared" si="0"/>
+        <v>0.53093327887200081</v>
+      </c>
+      <c r="E28" s="2">
+        <f t="shared" si="1"/>
+        <v>1.3656362465634222</v>
+      </c>
+      <c r="G28" s="1">
+        <v>0.23</v>
+      </c>
+      <c r="H28" s="2">
+        <v>0.28349353654225801</v>
+      </c>
+      <c r="I28" s="2">
+        <v>0.441721475193946</v>
+      </c>
+      <c r="J28" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52486802808777799</v>
+      </c>
+      <c r="K28" s="2">
+        <f t="shared" si="3"/>
+        <v>32.692043849722893</v>
+      </c>
+      <c r="M28" s="15">
+        <v>0.23</v>
+      </c>
+      <c r="N28" s="13">
+        <v>0.45808763919863699</v>
+      </c>
+      <c r="O28" s="13">
+        <v>0.26569222631349199</v>
+      </c>
+      <c r="P28" s="13">
+        <f t="shared" si="4"/>
+        <v>0.52956269157673908</v>
+      </c>
+      <c r="Q28" s="13">
+        <f t="shared" si="5"/>
+        <v>59.886136234569207</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A29" s="8">
+        <v>0.24</v>
+      </c>
+      <c r="B29" s="2">
+        <v>1.38722353279994E-2</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0.53107735126355704</v>
+      </c>
+      <c r="D29" s="2">
+        <f t="shared" si="0"/>
+        <v>0.53125849822672111</v>
+      </c>
+      <c r="E29" s="2">
+        <f t="shared" si="1"/>
+        <v>1.4962789116928121</v>
+      </c>
+      <c r="G29" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="H29" s="2">
+        <v>0.29162430450805898</v>
+      </c>
+      <c r="I29" s="2">
+        <v>0.43644020657844401</v>
+      </c>
+      <c r="J29" s="4">
+        <f t="shared" si="2"/>
+        <v>0.5249045521788166</v>
+      </c>
+      <c r="K29" s="2">
+        <f t="shared" si="3"/>
+        <v>33.75038860581715</v>
+      </c>
+      <c r="M29" s="8">
+        <v>0.24</v>
+      </c>
+      <c r="N29" s="2">
+        <v>0.46450449208163103</v>
+      </c>
+      <c r="O29" s="2">
+        <v>0.25068119905161601</v>
+      </c>
+      <c r="P29" s="2">
+        <f t="shared" si="4"/>
+        <v>0.52783092626519146</v>
+      </c>
+      <c r="Q29" s="2">
+        <f t="shared" si="5"/>
+        <v>61.645397863130924</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A30" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="B30" s="2">
+        <v>1.4268352104196601E-2</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0.531535482705631</v>
+      </c>
+      <c r="D30" s="2">
+        <f t="shared" si="0"/>
+        <v>0.53172695553909766</v>
+      </c>
+      <c r="E30" s="2">
+        <f t="shared" si="1"/>
+        <v>1.5376585481747653</v>
+      </c>
+      <c r="G30" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="H30" s="2">
+        <v>0.29929510262985098</v>
+      </c>
+      <c r="I30" s="2">
+        <v>0.43425057408607998</v>
+      </c>
+      <c r="J30" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52740034087238041</v>
+      </c>
+      <c r="K30" s="2">
+        <f t="shared" si="3"/>
+        <v>34.575470774812715</v>
+      </c>
+      <c r="M30" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="N30" s="5">
+        <v>0.47655304636780399</v>
+      </c>
+      <c r="O30" s="5">
+        <v>0.234544351408632</v>
+      </c>
+      <c r="P30" s="5">
+        <f t="shared" si="4"/>
+        <v>0.53114391531874883</v>
+      </c>
+      <c r="Q30" s="5">
+        <f t="shared" si="5"/>
+        <v>63.795046150674878</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A31" s="8">
+        <v>0.26</v>
+      </c>
+      <c r="B31" s="2">
+        <v>1.5730399012521702E-2</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0.53200407907812397</v>
+      </c>
+      <c r="D31" s="2">
+        <f t="shared" si="0"/>
+        <v>0.53223658800279405</v>
+      </c>
+      <c r="E31" s="2">
+        <f t="shared" si="1"/>
+        <v>1.6936391816935745</v>
+      </c>
+      <c r="G31" s="1">
+        <v>0.26</v>
+      </c>
+      <c r="H31" s="2">
+        <v>0.308471362684405</v>
+      </c>
+      <c r="I31" s="2">
+        <v>0.42997892544483501</v>
+      </c>
+      <c r="J31" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52918471059079997</v>
+      </c>
+      <c r="K31" s="2">
+        <f t="shared" si="3"/>
+        <v>35.656051297730151</v>
+      </c>
+      <c r="M31" s="15">
+        <v>0.26</v>
+      </c>
+      <c r="N31" s="13">
+        <v>0.48397917500777998</v>
+      </c>
+      <c r="O31" s="13">
+        <v>0.218488188505428</v>
+      </c>
+      <c r="P31" s="13">
+        <f t="shared" si="4"/>
+        <v>0.53101123373954595</v>
+      </c>
+      <c r="Q31" s="13">
+        <f t="shared" si="5"/>
+        <v>65.703617744243061</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A32" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="B32" s="2">
+        <v>1.65496295028431E-2</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0.53269863991816302</v>
+      </c>
+      <c r="D32" s="2">
+        <f t="shared" si="0"/>
+        <v>0.5329556559483557</v>
+      </c>
+      <c r="E32" s="2">
+        <f t="shared" si="1"/>
+        <v>1.779465829378968</v>
+      </c>
+      <c r="G32" s="1">
+        <v>0.27</v>
+      </c>
+      <c r="H32" s="2">
+        <v>0.318107592582969</v>
+      </c>
+      <c r="I32" s="2">
+        <v>0.42261564068045199</v>
+      </c>
+      <c r="J32" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52895786241125209</v>
+      </c>
+      <c r="K32" s="2">
+        <f t="shared" si="3"/>
+        <v>36.969191896965661</v>
+      </c>
+      <c r="M32" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="N32" s="2">
+        <v>0.491874081641899</v>
+      </c>
+      <c r="O32" s="2">
+        <v>0.19985504638325</v>
+      </c>
+      <c r="P32" s="2">
+        <f t="shared" si="4"/>
+        <v>0.53092574975782869</v>
+      </c>
+      <c r="Q32" s="2">
+        <f t="shared" si="5"/>
+        <v>67.887432169366392</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A33" s="8">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="B33" s="2">
+        <v>1.79666954531593E-2</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0.53307466411258897</v>
+      </c>
+      <c r="D33" s="2">
+        <f t="shared" si="0"/>
+        <v>0.53337735203536352</v>
+      </c>
+      <c r="E33" s="2">
+        <f t="shared" si="1"/>
+        <v>1.9303605417646563</v>
+      </c>
+      <c r="G33" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H33" s="2">
+        <v>0.32622939252014699</v>
+      </c>
+      <c r="I33" s="2">
+        <v>0.41682059404919702</v>
+      </c>
+      <c r="J33" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52930617242536449</v>
+      </c>
+      <c r="K33" s="2">
+        <f t="shared" si="3"/>
+        <v>38.048915457764323</v>
+      </c>
+      <c r="M33" s="8">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="N33" s="2">
+        <v>0.498804537374471</v>
+      </c>
+      <c r="O33" s="2">
+        <v>0.184835054150287</v>
+      </c>
+      <c r="P33" s="2">
+        <f t="shared" si="4"/>
+        <v>0.53194921162466213</v>
+      </c>
+      <c r="Q33" s="2">
+        <f t="shared" si="5"/>
+        <v>69.667506868445628</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A34" s="8">
+        <v>0.28999999999999898</v>
+      </c>
+      <c r="B34" s="2">
+        <v>1.8868364189676599E-2</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0.53368154692542602</v>
+      </c>
+      <c r="D34" s="2">
+        <f t="shared" si="0"/>
+        <v>0.5340149892052749</v>
+      </c>
+      <c r="E34" s="2">
+        <f t="shared" si="1"/>
+        <v>2.0248545883329818</v>
+      </c>
+      <c r="G34" s="1">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H34" s="2">
+        <v>0.33633456029134601</v>
+      </c>
+      <c r="I34" s="2">
+        <v>0.40687945117742902</v>
+      </c>
+      <c r="J34" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52789376226360063</v>
+      </c>
+      <c r="K34" s="2">
+        <f t="shared" si="3"/>
+        <v>39.577805311417968</v>
+      </c>
+      <c r="M34" s="8">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="N34" s="2">
+        <v>0.50562741345400197</v>
+      </c>
+      <c r="O34" s="2">
+        <v>0.163651827722395</v>
+      </c>
+      <c r="P34" s="2">
+        <f t="shared" si="4"/>
+        <v>0.53145178704475604</v>
+      </c>
+      <c r="Q34" s="2">
+        <f t="shared" si="5"/>
+        <v>72.065260212584377</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A35" s="8">
+        <v>0.29999999999999899</v>
+      </c>
+      <c r="B35" s="2">
+        <v>2.0551382745863898E-2</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0.53410399958348398</v>
+      </c>
+      <c r="D35" s="2">
+        <f t="shared" si="0"/>
+        <v>0.5344992438758368</v>
+      </c>
+      <c r="E35" s="2">
+        <f t="shared" si="1"/>
+        <v>2.2035537679834367</v>
+      </c>
+      <c r="G35" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="H35" s="2">
+        <v>0.344943234158405</v>
+      </c>
+      <c r="I35" s="2">
+        <v>0.39953410247029397</v>
+      </c>
+      <c r="J35" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52783835956512637</v>
+      </c>
+      <c r="K35" s="2">
+        <f t="shared" si="3"/>
+        <v>40.806133848758904</v>
+      </c>
+      <c r="M35" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="N35" s="2">
+        <v>0.511432048805464</v>
+      </c>
+      <c r="O35" s="2">
+        <v>0.14300013408625301</v>
+      </c>
+      <c r="P35" s="2">
+        <f t="shared" si="4"/>
+        <v>0.53104781224861553</v>
+      </c>
+      <c r="Q35" s="2">
+        <f t="shared" si="5"/>
+        <v>74.378619983773206</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A36" s="8">
+        <v>0.309999999999999</v>
+      </c>
+      <c r="B36" s="2">
+        <v>2.1944073175828398E-2</v>
+      </c>
+      <c r="C36" s="2">
+        <v>0.53479532117153195</v>
+      </c>
+      <c r="D36" s="2">
+        <f t="shared" si="0"/>
+        <v>0.53524534364579779</v>
+      </c>
+      <c r="E36" s="2">
+        <f t="shared" si="1"/>
+        <v>2.3496799787075844</v>
+      </c>
+      <c r="G36" s="1">
+        <v>0.31</v>
+      </c>
+      <c r="H36" s="2">
+        <v>0.35458843208559299</v>
+      </c>
+      <c r="I36" s="2">
+        <v>0.39268459572166298</v>
+      </c>
+      <c r="J36" s="4">
+        <f t="shared" si="2"/>
+        <v>0.5290880341550025</v>
+      </c>
+      <c r="K36" s="2">
+        <f t="shared" si="3"/>
+        <v>42.081573566732793</v>
+      </c>
+      <c r="M36" s="8">
+        <v>0.31</v>
+      </c>
+      <c r="N36" s="2">
+        <v>0.51878011984490502</v>
+      </c>
+      <c r="O36" s="2">
+        <v>0.122282808963993</v>
+      </c>
+      <c r="P36" s="2">
+        <f t="shared" si="4"/>
+        <v>0.53299709015567653</v>
+      </c>
+      <c r="Q36" s="2">
+        <f>DEGREES(ATAN(N36/O36))</f>
+        <v>76.736783883219815</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A37" s="8">
+        <v>0.31999999999999901</v>
+      </c>
+      <c r="B37" s="2">
+        <v>2.3728817804133301E-2</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0.53518297903038903</v>
+      </c>
+      <c r="D37" s="2">
+        <f t="shared" si="0"/>
+        <v>0.53570876214434238</v>
+      </c>
+      <c r="E37" s="2">
+        <f t="shared" si="1"/>
+        <v>2.538704188108909</v>
+      </c>
+      <c r="G37" s="1">
+        <v>0.32</v>
+      </c>
+      <c r="H37" s="2">
+        <v>0.36473843999991001</v>
+      </c>
+      <c r="I37" s="2">
+        <v>0.38531234292865701</v>
+      </c>
+      <c r="J37" s="4">
+        <f t="shared" si="2"/>
+        <v>0.53056548250591928</v>
+      </c>
+      <c r="K37" s="2">
+        <f t="shared" si="3"/>
+        <v>43.428769996050661</v>
+      </c>
+      <c r="M37" s="8">
+        <v>0.32</v>
+      </c>
+      <c r="N37" s="2">
+        <v>0.52560933375627705</v>
+      </c>
+      <c r="O37" s="2">
+        <v>0.10165192195853601</v>
+      </c>
+      <c r="P37" s="2">
+        <f t="shared" si="4"/>
+        <v>0.53534875078735522</v>
+      </c>
+      <c r="Q37" s="2">
+        <f t="shared" ref="Q37:Q39" si="6">DEGREES(ATAN(N37/O37))</f>
+        <v>79.054229553451393</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A38" s="8">
+        <v>0.32999999999999902</v>
+      </c>
+      <c r="B38" s="2">
+        <v>2.5529942947529902E-2</v>
+      </c>
+      <c r="C38" s="2">
+        <v>0.535664833482695</v>
+      </c>
+      <c r="D38" s="2">
+        <f t="shared" si="0"/>
+        <v>0.53627287067028429</v>
+      </c>
+      <c r="E38" s="2">
+        <f t="shared" si="1"/>
+        <v>2.7286688325851802</v>
+      </c>
+      <c r="G38" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="H38" s="2">
+        <v>0.37586219577398999</v>
+      </c>
+      <c r="I38" s="2">
+        <v>0.374839485983889</v>
+      </c>
+      <c r="J38" s="4">
+        <f t="shared" si="2"/>
+        <v>0.53082674241668659</v>
+      </c>
+      <c r="K38" s="2">
+        <f t="shared" si="3"/>
+        <v>45.078056197038222</v>
+      </c>
+      <c r="M38" s="8">
+        <v>0.33</v>
+      </c>
+      <c r="N38" s="2">
+        <v>0.53593605981300096</v>
+      </c>
+      <c r="O38" s="2">
+        <v>7.9079365032627996E-2</v>
+      </c>
+      <c r="P38" s="2">
+        <f t="shared" si="4"/>
+        <v>0.54173887268853815</v>
+      </c>
+      <c r="Q38" s="2">
+        <f t="shared" si="6"/>
+        <v>81.606360020152124</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A39" s="8">
+        <v>0.33999999999999903</v>
+      </c>
+      <c r="B39" s="2">
+        <v>2.7512139546923501E-2</v>
+      </c>
+      <c r="C39" s="2">
+        <v>0.53630577693671899</v>
+      </c>
+      <c r="D39" s="2">
+        <f t="shared" si="0"/>
+        <v>0.53701099076103387</v>
+      </c>
+      <c r="E39" s="2">
+        <f t="shared" si="1"/>
+        <v>2.936662179961143</v>
+      </c>
+      <c r="G39" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="H39" s="2">
+        <v>0.38677881858605401</v>
+      </c>
+      <c r="I39" s="2">
+        <v>0.36345047612497</v>
+      </c>
+      <c r="J39" s="4">
+        <f t="shared" si="2"/>
+        <v>0.53074862515346288</v>
+      </c>
+      <c r="K39" s="2">
+        <f t="shared" si="3"/>
+        <v>46.781035525860304</v>
+      </c>
+      <c r="M39" s="8">
+        <v>0.34</v>
+      </c>
+      <c r="N39" s="2">
+        <v>0.54452565366458905</v>
+      </c>
+      <c r="O39" s="2">
+        <v>5.5124076255154697E-2</v>
+      </c>
+      <c r="P39" s="2">
+        <f t="shared" si="4"/>
+        <v>0.54730873488537723</v>
+      </c>
+      <c r="Q39" s="2">
+        <f t="shared" si="6"/>
+        <v>84.219457665504621</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A40" s="8">
+        <v>0.34999999999999898</v>
+      </c>
+      <c r="B40" s="2">
+        <v>2.9678843509471399E-2</v>
+      </c>
+      <c r="C40" s="2">
+        <v>0.536785421229932</v>
+      </c>
+      <c r="D40" s="2">
+        <f t="shared" si="0"/>
+        <v>0.5376052661545041</v>
+      </c>
+      <c r="E40" s="2">
+        <f t="shared" si="1"/>
+        <v>3.164659113714468</v>
+      </c>
+      <c r="G40" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="H40" s="2">
+        <v>0.396983502975784</v>
+      </c>
+      <c r="I40" s="2">
+        <v>0.348260149978323</v>
+      </c>
+      <c r="J40" s="4">
+        <f t="shared" si="2"/>
+        <v>0.5280918799771952</v>
+      </c>
+      <c r="K40" s="2">
+        <f t="shared" si="3"/>
+        <v>48.740622403689947</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A41" s="8">
+        <v>0.35999999999999899</v>
+      </c>
+      <c r="B41" s="2">
+        <v>3.1962275090233402E-2</v>
+      </c>
+      <c r="C41" s="2">
+        <v>0.53738303598314996</v>
+      </c>
+      <c r="D41" s="2">
+        <f t="shared" si="0"/>
+        <v>0.5383327171846527</v>
+      </c>
+      <c r="E41" s="2">
+        <f t="shared" si="1"/>
+        <v>3.4038078038946993</v>
+      </c>
+      <c r="G41" s="1">
+        <v>0.36</v>
+      </c>
+      <c r="H41" s="2">
+        <v>0.40701692651799298</v>
+      </c>
+      <c r="I41" s="2">
+        <v>0.33420878298053602</v>
+      </c>
+      <c r="J41" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52664816442619855</v>
+      </c>
+      <c r="K41" s="2">
+        <f t="shared" si="3"/>
+        <v>50.609978028088108</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A42" s="8">
+        <v>0.369999999999999</v>
+      </c>
+      <c r="B42" s="2">
+        <v>3.7869681709684702E-2</v>
+      </c>
+      <c r="C42" s="2">
+        <v>0.52614316810265305</v>
+      </c>
+      <c r="D42" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52750426172106846</v>
+      </c>
+      <c r="E42" s="2">
+        <f t="shared" si="1"/>
+        <v>4.1168218075992185</v>
+      </c>
+      <c r="G42" s="1">
+        <v>0.37</v>
+      </c>
+      <c r="H42" s="2">
+        <v>0.41659934824481598</v>
+      </c>
+      <c r="I42" s="2">
+        <v>0.32376283012163898</v>
+      </c>
+      <c r="J42" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52761480942670547</v>
+      </c>
+      <c r="K42" s="2">
+        <f t="shared" si="3"/>
+        <v>52.147207697159018</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A43" s="8">
+        <v>0.37999999999999901</v>
+      </c>
+      <c r="B43" s="2">
+        <v>3.9899701953906498E-2</v>
+      </c>
+      <c r="C43" s="2">
+        <v>0.526005244847635</v>
+      </c>
+      <c r="D43" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52751635408130337</v>
+      </c>
+      <c r="E43" s="2">
+        <f t="shared" si="1"/>
+        <v>4.3378179612737604</v>
+      </c>
+      <c r="G43" s="1">
+        <v>0.38</v>
+      </c>
+      <c r="H43" s="2">
+        <v>0.42563211984139099</v>
+      </c>
+      <c r="I43" s="2">
+        <v>0.31127073322835602</v>
+      </c>
+      <c r="J43" s="4">
+        <f t="shared" si="2"/>
+        <v>0.5273065245236348</v>
+      </c>
+      <c r="K43" s="2">
+        <f t="shared" si="3"/>
+        <v>53.821472260179902</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A44" s="8">
+        <v>0.38999999999999901</v>
+      </c>
+      <c r="B44" s="2">
+        <v>4.3325251139050502E-2</v>
+      </c>
+      <c r="C44" s="2">
+        <v>0.52467765326253002</v>
+      </c>
+      <c r="D44" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52646340539427572</v>
+      </c>
+      <c r="E44" s="2">
+        <f t="shared" si="1"/>
+        <v>4.720488682226482</v>
+      </c>
+      <c r="G44" s="1">
+        <v>0.39</v>
+      </c>
+      <c r="H44" s="2">
+        <v>0.43664825927198703</v>
+      </c>
+      <c r="I44" s="2">
+        <v>0.29463254009455903</v>
+      </c>
+      <c r="J44" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52675424631209977</v>
+      </c>
+      <c r="K44" s="2">
+        <f t="shared" si="3"/>
+        <v>55.990119433250804</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A45" s="8">
+        <v>0.39999999999999902</v>
+      </c>
+      <c r="B45" s="2">
+        <v>4.5418192398049201E-2</v>
+      </c>
+      <c r="C45" s="2">
+        <v>0.52435619412193202</v>
+      </c>
+      <c r="D45" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52631951371267194</v>
+      </c>
+      <c r="E45" s="2">
+        <f t="shared" si="1"/>
+        <v>4.950436453509834</v>
+      </c>
+      <c r="G45" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="H45" s="5">
+        <v>0.44871885881995899</v>
+      </c>
+      <c r="I45" s="5">
+        <v>0.27951774495077197</v>
+      </c>
+      <c r="J45" s="7">
+        <f t="shared" si="2"/>
+        <v>0.52865752997857796</v>
+      </c>
+      <c r="K45" s="5">
+        <f t="shared" si="3"/>
+        <v>58.080230973195761</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A46" s="8">
+        <v>0.40999999999999898</v>
+      </c>
+      <c r="B46" s="2">
+        <v>4.7409659877447698E-2</v>
+      </c>
+      <c r="C46" s="2">
+        <v>0.52375635910261298</v>
+      </c>
+      <c r="D46" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52589770825714821</v>
+      </c>
+      <c r="E46" s="2">
+        <f t="shared" si="1"/>
+        <v>5.172234510420366</v>
+      </c>
+      <c r="G46" s="1">
+        <v>0.41</v>
+      </c>
+      <c r="H46" s="2">
+        <v>0.459221220234802</v>
+      </c>
+      <c r="I46" s="2">
+        <v>0.26288851984559902</v>
+      </c>
+      <c r="J46" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52914506799227601</v>
+      </c>
+      <c r="K46" s="2">
+        <f t="shared" si="3"/>
+        <v>60.210331332474446</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A47" s="8">
+        <v>0.41999999999999899</v>
+      </c>
+      <c r="B47" s="2">
+        <v>4.8324197184934102E-2</v>
+      </c>
+      <c r="C47" s="2">
+        <v>0.52322010881321301</v>
+      </c>
+      <c r="D47" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52544696240446465</v>
+      </c>
+      <c r="E47" s="2">
+        <f t="shared" si="1"/>
+        <v>5.2768228902621983</v>
+      </c>
+      <c r="G47" s="1">
+        <v>0.42</v>
+      </c>
+      <c r="H47" s="2">
+        <v>0.46814637548789401</v>
+      </c>
+      <c r="I47" s="2">
+        <v>0.244231086763287</v>
+      </c>
+      <c r="J47" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52802448108400091</v>
+      </c>
+      <c r="K47" s="2">
+        <f t="shared" si="3"/>
+        <v>62.449035146803688</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A48" s="8">
+        <v>0.42999999999999899</v>
+      </c>
+      <c r="B48" s="2">
+        <v>5.0257127383274897E-2</v>
+      </c>
+      <c r="C48" s="2">
+        <v>0.52254960081583501</v>
+      </c>
+      <c r="D48" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52496082155300627</v>
+      </c>
+      <c r="E48" s="2">
+        <f t="shared" si="1"/>
+        <v>5.493625376317623</v>
+      </c>
+      <c r="G48" s="1">
+        <v>0.43</v>
+      </c>
+      <c r="H48" s="2">
+        <v>0.48215550272676699</v>
+      </c>
+      <c r="I48" s="2">
+        <v>0.22240130530022401</v>
+      </c>
+      <c r="J48" s="4">
+        <f t="shared" si="2"/>
+        <v>0.53097671268045721</v>
+      </c>
+      <c r="K48" s="2">
+        <f t="shared" si="3"/>
+        <v>65.237792438546421</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A49" s="8">
+        <v>0.439999999999999</v>
+      </c>
+      <c r="B49" s="2">
+        <v>5.2546608874460998E-2</v>
+      </c>
+      <c r="C49" s="2">
+        <v>0.52196562370204802</v>
+      </c>
+      <c r="D49" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52460390622914121</v>
+      </c>
+      <c r="E49" s="2">
+        <f t="shared" si="1"/>
+        <v>5.7486345121703994</v>
+      </c>
+      <c r="G49" s="12">
+        <v>0.44</v>
+      </c>
+      <c r="H49" s="13">
+        <v>0.49362264397275002</v>
+      </c>
+      <c r="I49" s="13">
+        <v>0.202157698027537</v>
+      </c>
+      <c r="J49" s="14">
+        <f t="shared" si="2"/>
+        <v>0.53341451940722528</v>
+      </c>
+      <c r="K49" s="13">
+        <f t="shared" si="3"/>
+        <v>67.728989316549189</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A50" s="8">
+        <v>0.44999999999999901</v>
+      </c>
+      <c r="B50" s="2">
+        <v>5.4724894944489601E-2</v>
+      </c>
+      <c r="C50" s="2">
+        <v>0.523565146725405</v>
+      </c>
+      <c r="D50" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52641739807141663</v>
+      </c>
+      <c r="E50" s="2">
+        <f t="shared" si="1"/>
+        <v>5.9670914999119553</v>
+      </c>
+      <c r="G50" s="12">
+        <v>0.45</v>
+      </c>
+      <c r="H50" s="13">
+        <v>0.50452219903123896</v>
+      </c>
+      <c r="I50" s="13">
+        <v>0.17884039068895899</v>
+      </c>
+      <c r="J50" s="14">
+        <f t="shared" si="2"/>
+        <v>0.53528173390944012</v>
+      </c>
+      <c r="K50" s="13">
+        <f t="shared" si="3"/>
+        <v>70.48186746907048</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A51" s="8">
+        <v>0.46</v>
+      </c>
+      <c r="B51" s="2">
+        <v>5.6654305163715897E-2</v>
+      </c>
+      <c r="C51" s="2">
+        <v>0.52262656839934096</v>
+      </c>
+      <c r="D51" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52568834901532147</v>
+      </c>
+      <c r="E51" s="2">
+        <f t="shared" si="1"/>
+        <v>6.1868773112401305</v>
+      </c>
+      <c r="G51" s="12">
+        <v>0.46</v>
+      </c>
+      <c r="H51" s="13">
+        <v>0.51745893009548904</v>
+      </c>
+      <c r="I51" s="13">
+        <v>0.15445965520438201</v>
+      </c>
+      <c r="J51" s="14">
+        <f t="shared" si="2"/>
+        <v>0.54001993428152706</v>
+      </c>
+      <c r="K51" s="13">
+        <f t="shared" si="3"/>
+        <v>73.37982228622559</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A52" s="8">
+        <v>0.47</v>
+      </c>
+      <c r="B52" s="2">
+        <v>6.0927095968718002E-2</v>
+      </c>
+      <c r="C52" s="2">
+        <v>0.52341012605634196</v>
+      </c>
+      <c r="D52" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52694427701750135</v>
+      </c>
+      <c r="E52" s="2">
+        <f t="shared" si="1"/>
+        <v>6.6395838732926427</v>
+      </c>
+      <c r="G52" s="1">
+        <v>0.47</v>
+      </c>
+      <c r="H52" s="2">
+        <v>0.52832261303948302</v>
+      </c>
+      <c r="I52" s="2">
+        <v>0.12908723580279399</v>
+      </c>
+      <c r="J52" s="4">
+        <f t="shared" si="2"/>
+        <v>0.54386422744658747</v>
+      </c>
+      <c r="K52" s="2">
+        <f t="shared" si="3"/>
+        <v>76.269697065627881</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A53" s="8">
+        <v>0.48</v>
+      </c>
+      <c r="B53" s="2">
+        <v>6.4298045216000604E-2</v>
+      </c>
+      <c r="C53" s="2">
+        <v>0.52248452175150595</v>
+      </c>
+      <c r="D53" s="2">
+        <f t="shared" si="0"/>
+        <v>0.5264259815857294</v>
+      </c>
+      <c r="E53" s="2">
+        <f t="shared" si="1"/>
+        <v>7.0156654138898853</v>
+      </c>
+      <c r="G53" s="1">
+        <v>0.48</v>
+      </c>
+      <c r="H53" s="2">
+        <v>0.534616102013447</v>
+      </c>
+      <c r="I53" s="2">
+        <v>0.106878196753334</v>
+      </c>
+      <c r="J53" s="4">
+        <f t="shared" si="2"/>
+        <v>0.54519475921297766</v>
+      </c>
+      <c r="K53" s="2">
+        <f t="shared" si="3"/>
+        <v>78.694707280294082</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A54" s="8">
+        <v>0.49</v>
+      </c>
+      <c r="B54" s="2">
+        <v>6.6234484690438494E-2</v>
+      </c>
+      <c r="C54" s="2">
+        <v>0.52146092969011004</v>
+      </c>
+      <c r="D54" s="2">
+        <f t="shared" si="0"/>
+        <v>0.5256505570771155</v>
+      </c>
+      <c r="E54" s="2">
+        <f t="shared" si="1"/>
+        <v>7.2387844576299347</v>
+      </c>
+      <c r="G54" s="1">
+        <v>0.49</v>
+      </c>
+      <c r="H54" s="2">
+        <v>0.53899631703294903</v>
+      </c>
+      <c r="I54" s="2">
+        <v>8.0058326698925805E-2</v>
+      </c>
+      <c r="J54" s="4">
+        <f t="shared" si="2"/>
+        <v>0.5449095020725141</v>
+      </c>
+      <c r="K54" s="2">
+        <f t="shared" si="3"/>
+        <v>81.551498343291598</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A55" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="B55" s="2">
+        <v>7.2965919111353902E-2</v>
+      </c>
+      <c r="C55" s="2">
+        <v>0.52187646094270201</v>
+      </c>
+      <c r="D55" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52695262200490489</v>
+      </c>
+      <c r="E55" s="2">
+        <f t="shared" si="1"/>
+        <v>7.9591885137184226</v>
+      </c>
+      <c r="G55" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="H55" s="13">
+        <v>0.55056635732742798</v>
+      </c>
+      <c r="I55" s="13">
+        <v>4.9039114044486402E-2</v>
+      </c>
+      <c r="J55" s="14">
+        <f t="shared" si="2"/>
+        <v>0.55274600724660261</v>
+      </c>
+      <c r="K55" s="13">
+        <f t="shared" si="3"/>
+        <v>84.910079342528221</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A56" s="8">
+        <v>0.51</v>
+      </c>
+      <c r="B56" s="2">
+        <v>7.6538469909974399E-2</v>
+      </c>
+      <c r="C56" s="2">
+        <v>0.52084532066156197</v>
+      </c>
+      <c r="D56" s="2">
+        <f t="shared" si="0"/>
+        <v>0.5264389664825404</v>
+      </c>
+      <c r="E56" s="2">
+        <f t="shared" si="1"/>
+        <v>8.359809812032081</v>
+      </c>
+      <c r="G56" s="1"/>
+      <c r="J56" s="4"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A57" s="8">
+        <v>0.52</v>
+      </c>
+      <c r="B57" s="2">
+        <v>7.4776471863669203E-2</v>
+      </c>
+      <c r="C57" s="2">
+        <v>0.52093133261251201</v>
+      </c>
+      <c r="D57" s="2">
+        <f t="shared" si="0"/>
+        <v>0.5262708181552781</v>
+      </c>
+      <c r="E57" s="2">
+        <f t="shared" si="1"/>
+        <v>8.1686553001992284</v>
+      </c>
+      <c r="G57" s="1"/>
+      <c r="J57" s="4"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A58" s="8">
+        <v>0.53</v>
+      </c>
+      <c r="B58" s="2">
+        <v>7.7948924375624604E-2</v>
+      </c>
+      <c r="C58" s="2">
+        <v>0.51950566972642098</v>
+      </c>
+      <c r="D58" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52532102155654692</v>
+      </c>
+      <c r="E58" s="2">
+        <f t="shared" si="1"/>
+        <v>8.5332543957113387</v>
+      </c>
+      <c r="G58" s="1"/>
+      <c r="J58" s="4"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A59" s="8">
+        <v>0.54</v>
+      </c>
+      <c r="B59" s="2">
+        <v>7.9767447518746495E-2</v>
+      </c>
+      <c r="C59" s="2">
+        <v>0.51901716477971305</v>
+      </c>
+      <c r="D59" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52511109588317384</v>
+      </c>
+      <c r="E59" s="2">
+        <f t="shared" si="1"/>
+        <v>8.7373895557329249</v>
+      </c>
+      <c r="G59" s="1"/>
+      <c r="J59" s="4"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A60" s="8">
+        <v>0.54999999999999905</v>
+      </c>
+      <c r="B60" s="2">
+        <v>8.3646293342997599E-2</v>
+      </c>
+      <c r="C60" s="2">
+        <v>0.51783533308080898</v>
+      </c>
+      <c r="D60" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52454755225521277</v>
+      </c>
+      <c r="E60" s="2">
+        <f t="shared" si="1"/>
+        <v>9.1757688141176441</v>
+      </c>
+      <c r="G60" s="8"/>
+      <c r="J60" s="4"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A61" s="8">
+        <v>0.55999999999999905</v>
+      </c>
+      <c r="B61" s="2">
+        <v>8.7065451263653504E-2</v>
+      </c>
+      <c r="C61" s="2">
+        <v>0.51843301514332796</v>
+      </c>
+      <c r="D61" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52569305111856457</v>
+      </c>
+      <c r="E61" s="2">
+        <f t="shared" si="1"/>
+        <v>9.5332719955656415</v>
+      </c>
+      <c r="G61" s="8"/>
+      <c r="J61" s="4"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A62" s="8">
+        <v>0.56999999999999895</v>
+      </c>
+      <c r="B62" s="2">
+        <v>9.4953732811302899E-2</v>
+      </c>
+      <c r="C62" s="2">
+        <v>0.51302945709980297</v>
+      </c>
+      <c r="D62" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52174269063104173</v>
+      </c>
+      <c r="E62" s="2">
+        <f t="shared" si="1"/>
+        <v>10.48589203518474</v>
+      </c>
+      <c r="G62" s="1"/>
+      <c r="J62" s="4"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A63" s="8">
+        <v>0.57999999999999896</v>
+      </c>
+      <c r="B63" s="2">
+        <v>9.2481168738986999E-2</v>
+      </c>
+      <c r="C63" s="2">
+        <v>0.51468438338579503</v>
+      </c>
+      <c r="D63" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52292712787973139</v>
+      </c>
+      <c r="E63" s="2">
+        <f t="shared" si="1"/>
+        <v>10.186502357339206</v>
+      </c>
+      <c r="G63" s="1"/>
+      <c r="J63" s="4"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A64" s="8">
+        <v>0.58999999999999897</v>
+      </c>
+      <c r="B64" s="2">
+        <v>9.3724831566238606E-2</v>
+      </c>
+      <c r="C64" s="2">
+        <v>0.52018377836837204</v>
+      </c>
+      <c r="D64" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52855984271387413</v>
+      </c>
+      <c r="E64" s="2">
+        <f t="shared" si="1"/>
+        <v>10.213762251263265</v>
+      </c>
+      <c r="G64" s="1"/>
+      <c r="J64" s="4"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A65" s="8">
+        <v>0.59999999999999898</v>
+      </c>
+      <c r="B65" s="2">
+        <v>0.10209417096453</v>
+      </c>
+      <c r="C65" s="2">
+        <v>0.51588687532930599</v>
+      </c>
+      <c r="D65" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52589208767766182</v>
+      </c>
+      <c r="E65" s="2">
+        <f t="shared" si="1"/>
+        <v>11.194209411851357</v>
+      </c>
+      <c r="G65" s="1"/>
+      <c r="J65" s="4"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A66" s="8">
+        <v>0.60999999999999899</v>
+      </c>
+      <c r="B66" s="2">
+        <v>0.104778118529777</v>
+      </c>
+      <c r="C66" s="2">
+        <v>0.51264268930009305</v>
+      </c>
+      <c r="D66" s="2">
+        <f t="shared" si="0"/>
+        <v>0.5232408441773938</v>
+      </c>
+      <c r="E66" s="2">
+        <f t="shared" si="1"/>
+        <v>11.551482552605684</v>
+      </c>
+      <c r="G66" s="1"/>
+      <c r="J66" s="4"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A67" s="8">
+        <v>0.619999999999999</v>
+      </c>
+      <c r="B67" s="2">
+        <v>0.111194757070946</v>
+      </c>
+      <c r="C67" s="2">
+        <v>0.51390097397924905</v>
+      </c>
+      <c r="D67" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52579319609223496</v>
+      </c>
+      <c r="E67" s="2">
+        <f t="shared" si="1"/>
+        <v>12.209099467575069</v>
+      </c>
+      <c r="G67" s="1"/>
+      <c r="J67" s="3"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A68" s="8">
+        <v>0.62999999999999901</v>
+      </c>
+      <c r="B68" s="2">
+        <v>0.114791951403157</v>
+      </c>
+      <c r="C68" s="2">
+        <v>0.51064084716842295</v>
+      </c>
+      <c r="D68" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52338443509893318</v>
+      </c>
+      <c r="E68" s="2">
+        <f t="shared" si="1"/>
+        <v>12.669464175415371</v>
+      </c>
+      <c r="G68" s="1"/>
+      <c r="J68" s="3"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A69" s="8">
+        <v>0.63999999999999901</v>
+      </c>
+      <c r="B69" s="2">
+        <v>0.119001649575421</v>
+      </c>
+      <c r="C69" s="2">
+        <v>0.50935108721085998</v>
+      </c>
+      <c r="D69" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52306779928089286</v>
+      </c>
+      <c r="E69" s="2">
+        <f t="shared" si="1"/>
+        <v>13.150349884620448</v>
+      </c>
+      <c r="G69" s="1"/>
+      <c r="J69" s="3"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A70" s="8">
+        <v>0.64999999999999902</v>
+      </c>
+      <c r="B70" s="2">
+        <v>0.123419973344478</v>
+      </c>
+      <c r="C70" s="2">
+        <v>0.50774966944220901</v>
+      </c>
+      <c r="D70" s="2">
+        <f t="shared" ref="D70:D120" si="7">(B70^2+C70^2)^0.5</f>
+        <v>0.52253441670288492</v>
+      </c>
+      <c r="E70" s="2">
+        <f t="shared" ref="E70:E120" si="8">DEGREES(ATAN(B70/C70))</f>
+        <v>13.662069522404304</v>
+      </c>
+      <c r="G70" s="1"/>
+      <c r="J70" s="3"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A71" s="8">
+        <v>0.65999999999999903</v>
+      </c>
+      <c r="B71" s="2">
+        <v>0.127529583795817</v>
+      </c>
+      <c r="C71" s="2">
+        <v>0.50767793592495103</v>
+      </c>
+      <c r="D71" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52345074397516433</v>
+      </c>
+      <c r="E71" s="2">
+        <f t="shared" si="8"/>
+        <v>14.101029790223093</v>
+      </c>
+      <c r="G71" s="1"/>
+      <c r="J71" s="3"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A72" s="8">
+        <v>0.66999999999999904</v>
+      </c>
+      <c r="B72" s="2">
+        <v>0.13163122385634901</v>
+      </c>
+      <c r="C72" s="2">
+        <v>0.50714957902421098</v>
+      </c>
+      <c r="D72" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52395369508989498</v>
+      </c>
+      <c r="E72" s="2">
+        <f t="shared" si="8"/>
+        <v>14.550121308007204</v>
+      </c>
+      <c r="G72" s="1"/>
+      <c r="J72" s="3"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A73" s="8">
+        <v>0.67999999999999905</v>
+      </c>
+      <c r="B73" s="2">
+        <v>0.13571692313526901</v>
+      </c>
+      <c r="C73" s="2">
+        <v>0.50570797535650702</v>
+      </c>
+      <c r="D73" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52360255878336004</v>
+      </c>
+      <c r="E73" s="2">
+        <f t="shared" si="8"/>
+        <v>15.022500831596743</v>
+      </c>
+      <c r="G73" s="1"/>
+      <c r="J73" s="3"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A74" s="8">
+        <v>0.68999999999999895</v>
+      </c>
+      <c r="B74" s="2">
+        <v>0.14118046295544101</v>
+      </c>
+      <c r="C74" s="2">
+        <v>0.50469908389986595</v>
+      </c>
+      <c r="D74" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52407355248063858</v>
+      </c>
+      <c r="E74" s="2">
+        <f t="shared" si="8"/>
+        <v>15.628004300147362</v>
+      </c>
+      <c r="G74" s="1"/>
+      <c r="J74" s="3"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A75" s="8">
+        <v>0.69999999999999896</v>
+      </c>
+      <c r="B75" s="2">
+        <v>0.14665197316642001</v>
+      </c>
+      <c r="C75" s="2">
+        <v>0.50414681582670695</v>
+      </c>
+      <c r="D75" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52504362975072083</v>
+      </c>
+      <c r="E75" s="2">
+        <f t="shared" si="8"/>
+        <v>16.219259175006968</v>
+      </c>
+      <c r="G75" s="1"/>
+      <c r="J75" s="3"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A76" s="8">
+        <v>0.71</v>
+      </c>
+      <c r="B76" s="2">
+        <v>0.151178355047208</v>
+      </c>
+      <c r="C76" s="2">
+        <v>0.50178399500123205</v>
+      </c>
+      <c r="D76" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52406304265248105</v>
+      </c>
+      <c r="E76" s="2">
+        <f t="shared" si="8"/>
+        <v>16.766595016246715</v>
+      </c>
+      <c r="G76" s="1"/>
+      <c r="J76" s="3"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A77" s="8">
+        <v>0.72</v>
+      </c>
+      <c r="B77" s="2">
+        <v>0.15753920085273199</v>
+      </c>
+      <c r="C77" s="2">
+        <v>0.49984591599601402</v>
+      </c>
+      <c r="D77" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52408447748737197</v>
+      </c>
+      <c r="E77" s="2">
+        <f t="shared" si="8"/>
+        <v>17.493576086142252</v>
+      </c>
+      <c r="G77" s="1"/>
+      <c r="J77" s="3"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A78" s="8">
+        <v>0.73</v>
+      </c>
+      <c r="B78" s="2">
+        <v>0.16345139366558001</v>
+      </c>
+      <c r="C78" s="2">
+        <v>0.49837243076508397</v>
+      </c>
+      <c r="D78" s="2">
+        <f t="shared" si="7"/>
+        <v>0.5244915993969006</v>
+      </c>
+      <c r="E78" s="2">
+        <f t="shared" si="8"/>
+        <v>18.157958008099556</v>
+      </c>
+      <c r="G78" s="1"/>
+      <c r="J78" s="3"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A79" s="8">
+        <v>0.74</v>
+      </c>
+      <c r="B79" s="2">
+        <v>0.16981223947110299</v>
+      </c>
+      <c r="C79" s="2">
+        <v>0.496434351759866</v>
+      </c>
+      <c r="D79" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52467443456054685</v>
+      </c>
+      <c r="E79" s="2">
+        <f t="shared" si="8"/>
+        <v>18.883962513676796</v>
+      </c>
+      <c r="G79" s="1"/>
+      <c r="J79" s="3"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A80" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="B80" s="2">
+        <v>0.176613767878496</v>
+      </c>
+      <c r="C80" s="2">
+        <v>0.49357505559687698</v>
+      </c>
+      <c r="D80" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52422205076827844</v>
+      </c>
+      <c r="E80" s="2">
+        <f t="shared" si="8"/>
+        <v>19.688507372802363</v>
+      </c>
+      <c r="G80" s="1"/>
+      <c r="J80" s="3"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A81" s="8">
+        <v>0.76</v>
+      </c>
+      <c r="B81" s="2">
+        <v>0.182990554465632</v>
+      </c>
+      <c r="C81" s="2">
+        <v>0.49255022335862297</v>
+      </c>
+      <c r="D81" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52544387478994248</v>
+      </c>
+      <c r="E81" s="2">
+        <f t="shared" si="8"/>
+        <v>20.380864238324229</v>
+      </c>
+      <c r="G81" s="1"/>
+      <c r="J81" s="3"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A82" s="8">
+        <v>0.77</v>
+      </c>
+      <c r="B82" s="2">
+        <v>0.19071330003079601</v>
+      </c>
+      <c r="C82" s="2">
+        <v>0.49013160979750298</v>
+      </c>
+      <c r="D82" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52592828192761043</v>
+      </c>
+      <c r="E82" s="2">
+        <f t="shared" si="8"/>
+        <v>21.26132533066604</v>
+      </c>
+      <c r="G82" s="1"/>
+      <c r="J82" s="3"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A83" s="8">
+        <v>0.78</v>
+      </c>
+      <c r="B83" s="2">
+        <v>0.19660955206203101</v>
+      </c>
+      <c r="C83" s="2">
+        <v>0.48774487779960901</v>
+      </c>
+      <c r="D83" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52588057749054395</v>
+      </c>
+      <c r="E83" s="2">
+        <f t="shared" si="8"/>
+        <v>21.954322404420065</v>
+      </c>
+      <c r="G83" s="1"/>
+      <c r="J83" s="3"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A84" s="8">
+        <v>0.79</v>
+      </c>
+      <c r="B84" s="2">
+        <v>0.20434026801800001</v>
+      </c>
+      <c r="C84" s="2">
+        <v>0.48578288762197203</v>
+      </c>
+      <c r="D84" s="2">
+        <f t="shared" si="7"/>
+        <v>0.5270103974685979</v>
+      </c>
+      <c r="E84" s="2">
+        <f t="shared" si="8"/>
+        <v>22.813624916249957</v>
+      </c>
+      <c r="G84" s="1"/>
+      <c r="J84" s="3"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A85" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="B85" s="2">
+        <v>0.21250369618503301</v>
+      </c>
+      <c r="C85" s="2">
+        <v>0.48244305690308198</v>
+      </c>
+      <c r="D85" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52717086797953017</v>
+      </c>
+      <c r="E85" s="2">
+        <f t="shared" si="8"/>
+        <v>23.772250974545017</v>
+      </c>
+      <c r="G85" s="1"/>
+      <c r="J85" s="3"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A86" s="8">
+        <v>0.81</v>
+      </c>
+      <c r="B86" s="2">
+        <v>0.220643213179646</v>
+      </c>
+      <c r="C86" s="2">
+        <v>0.477733356033745</v>
+      </c>
+      <c r="D86" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52622484451943508</v>
+      </c>
+      <c r="E86" s="2">
+        <f t="shared" si="8"/>
+        <v>24.790057950086311</v>
+      </c>
+      <c r="G86" s="1"/>
+      <c r="J86" s="3"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A87" s="8">
+        <v>0.81999999999999895</v>
+      </c>
+      <c r="B87" s="2">
+        <v>0.228326106790777</v>
+      </c>
+      <c r="C87" s="2">
+        <v>0.473031625555215</v>
+      </c>
+      <c r="D87" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52525396696992444</v>
+      </c>
+      <c r="E87" s="2">
+        <f t="shared" si="8"/>
+        <v>25.765988816564249</v>
+      </c>
+      <c r="G87" s="1"/>
+      <c r="J87" s="3"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A88" s="8">
+        <v>0.82999999999999896</v>
+      </c>
+      <c r="B88" s="2">
+        <v>0.23282857749914701</v>
+      </c>
+      <c r="C88" s="2">
+        <v>0.469298934579294</v>
+      </c>
+      <c r="D88" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52388036468027388</v>
+      </c>
+      <c r="E88" s="2">
+        <f t="shared" si="8"/>
+        <v>26.38692823279403</v>
+      </c>
+      <c r="G88" s="1"/>
+      <c r="J88" s="3"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A89" s="8">
+        <v>0.84</v>
+      </c>
+      <c r="B89" s="2">
+        <v>0.241440658658855</v>
+      </c>
+      <c r="C89" s="2">
+        <v>0.46549451008611598</v>
+      </c>
+      <c r="D89" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52438414409088963</v>
+      </c>
+      <c r="E89" s="2">
+        <f t="shared" si="8"/>
+        <v>27.414669430142009</v>
+      </c>
+      <c r="G89" s="1"/>
+      <c r="J89" s="3"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A90" s="8">
+        <v>0.84999999999999898</v>
+      </c>
+      <c r="B90" s="2">
+        <v>0.25139072840578403</v>
+      </c>
+      <c r="C90" s="2">
+        <v>0.459839680886589</v>
+      </c>
+      <c r="D90" s="2">
+        <f t="shared" si="7"/>
+        <v>0.5240704441640176</v>
+      </c>
+      <c r="E90" s="2">
+        <f t="shared" si="8"/>
+        <v>28.665079764979023</v>
+      </c>
+      <c r="G90" s="1"/>
+      <c r="J90" s="3"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A91" s="8">
+        <v>0.86</v>
+      </c>
+      <c r="B91" s="2">
+        <v>0.26091605633245601</v>
+      </c>
+      <c r="C91" s="2">
+        <v>0.45601931561179798</v>
+      </c>
+      <c r="D91" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52538633848163008</v>
+      </c>
+      <c r="E91" s="2">
+        <f t="shared" si="8"/>
+        <v>29.776467586577013</v>
+      </c>
+      <c r="G91" s="1"/>
+      <c r="J91" s="3"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A92" s="8">
+        <v>0.869999999999999</v>
+      </c>
+      <c r="B92" s="2">
+        <v>0.26994490892161399</v>
+      </c>
+      <c r="C92" s="2">
+        <v>0.44992380381040198</v>
+      </c>
+      <c r="D92" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52469198877810164</v>
+      </c>
+      <c r="E92" s="2">
+        <f t="shared" si="8"/>
+        <v>30.962878835795767</v>
+      </c>
+      <c r="G92" s="1"/>
+      <c r="J92" s="3"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A93" s="8">
+        <v>0.88</v>
+      </c>
+      <c r="B93" s="2">
+        <v>0.27989497866854302</v>
+      </c>
+      <c r="C93" s="2">
+        <v>0.444268974610876</v>
+      </c>
+      <c r="D93" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52508677462459796</v>
+      </c>
+      <c r="E93" s="2">
+        <f t="shared" si="8"/>
+        <v>32.211437776008395</v>
+      </c>
+      <c r="G93" s="1"/>
+      <c r="J93" s="3"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A94" s="8">
+        <v>0.88999999999999901</v>
+      </c>
+      <c r="B94" s="2">
+        <v>0.28983707802466502</v>
+      </c>
+      <c r="C94" s="2">
+        <v>0.43815752202786801</v>
+      </c>
+      <c r="D94" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52534516834884604</v>
+      </c>
+      <c r="E94" s="2">
+        <f t="shared" si="8"/>
+        <v>33.484260913738005</v>
+      </c>
+      <c r="G94" s="1"/>
+      <c r="J94" s="3"/>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A95" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="B95" s="2">
+        <v>0.29748011968176402</v>
+      </c>
+      <c r="C95" s="2">
+        <v>0.43117267463192699</v>
+      </c>
+      <c r="D95" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52383613559502196</v>
+      </c>
+      <c r="E95" s="2">
+        <f t="shared" si="8"/>
+        <v>34.603062465654773</v>
+      </c>
+      <c r="G95" s="1"/>
+      <c r="J95" s="3"/>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A96" s="8">
+        <v>0.90999999999999903</v>
+      </c>
+      <c r="B96" s="2">
+        <v>0.30925668296262099</v>
+      </c>
+      <c r="C96" s="2">
+        <v>0.42548596386917498</v>
+      </c>
+      <c r="D96" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52600190247443401</v>
+      </c>
+      <c r="E96" s="2">
+        <f t="shared" si="8"/>
+        <v>36.010842317995042</v>
+      </c>
+      <c r="G96" s="1"/>
+      <c r="J96" s="3"/>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A97" s="8">
+        <v>0.92</v>
+      </c>
+      <c r="B97" s="2">
+        <v>0.318710277372036</v>
+      </c>
+      <c r="C97" s="2">
+        <v>0.41755598814304501</v>
+      </c>
+      <c r="D97" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52528967640405311</v>
+      </c>
+      <c r="E97" s="2">
+        <f t="shared" si="8"/>
+        <v>37.353608930827704</v>
+      </c>
+      <c r="G97" s="1"/>
+      <c r="J97" s="3"/>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A98" s="8">
+        <v>0.92999999999999905</v>
+      </c>
+      <c r="B98" s="2">
+        <v>0.32817184217225698</v>
+      </c>
+      <c r="C98" s="2">
+        <v>0.410082635800397</v>
+      </c>
+      <c r="D98" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52522807063192445</v>
+      </c>
+      <c r="E98" s="2">
+        <f t="shared" si="8"/>
+        <v>38.668814950436705</v>
+      </c>
+      <c r="G98" s="1"/>
+      <c r="J98" s="3"/>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A99" s="8">
+        <v>0.94</v>
+      </c>
+      <c r="B99" s="2">
+        <v>0.342600471455136</v>
+      </c>
+      <c r="C99" s="2">
+        <v>0.39932524547450299</v>
+      </c>
+      <c r="D99" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52615181717309834</v>
+      </c>
+      <c r="E99" s="2">
+        <f t="shared" si="8"/>
+        <v>40.627891923331845</v>
+      </c>
+      <c r="G99" s="1"/>
+      <c r="J99" s="3"/>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A100" s="8">
+        <v>0.94999999999999896</v>
+      </c>
+      <c r="B100" s="2">
+        <v>0.35294340145909597</v>
+      </c>
+      <c r="C100" s="2">
+        <v>0.39000945881631399</v>
+      </c>
+      <c r="D100" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52600040171059825</v>
+      </c>
+      <c r="E100" s="2">
+        <f t="shared" si="8"/>
+        <v>42.143870921967959</v>
+      </c>
+      <c r="G100" s="1"/>
+      <c r="J100" s="3"/>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A101" s="8">
+        <v>0.95999999999999897</v>
+      </c>
+      <c r="B101" s="2">
+        <v>0.36644284319339798</v>
+      </c>
+      <c r="C101" s="2">
+        <v>0.378354762505069</v>
+      </c>
+      <c r="D101" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52671878990399457</v>
+      </c>
+      <c r="E101" s="2">
+        <f t="shared" si="8"/>
+        <v>44.083718162815103</v>
+      </c>
+      <c r="G101" s="1"/>
+      <c r="J101" s="3"/>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A102" s="8">
+        <v>0.96999999999999897</v>
+      </c>
+      <c r="B102" s="2">
+        <v>0.37811579139377099</v>
+      </c>
+      <c r="C102" s="2">
+        <v>0.36673194775704998</v>
+      </c>
+      <c r="D102" s="2">
+        <f t="shared" si="7"/>
+        <v>0.5267483964921178</v>
+      </c>
+      <c r="E102" s="2">
+        <f t="shared" si="8"/>
+        <v>45.87560904481267</v>
+      </c>
+      <c r="G102" s="1"/>
+      <c r="J102" s="3"/>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A103" s="8">
+        <v>0.97999999999999898</v>
+      </c>
+      <c r="B103" s="2">
+        <v>0.39071792714272202</v>
+      </c>
+      <c r="C103" s="2">
+        <v>0.356006438994382</v>
+      </c>
+      <c r="D103" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52858403607767623</v>
+      </c>
+      <c r="E103" s="2">
+        <f t="shared" si="8"/>
+        <v>47.661478849397675</v>
+      </c>
+      <c r="G103" s="1"/>
+      <c r="J103" s="3"/>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A104" s="8">
+        <v>0.98999999999999899</v>
+      </c>
+      <c r="B104" s="2">
+        <v>0.400099788034878</v>
+      </c>
+      <c r="C104" s="2">
+        <v>0.34396685281691303</v>
+      </c>
+      <c r="D104" s="2">
+        <f t="shared" si="7"/>
+        <v>0.5276296392568619</v>
+      </c>
+      <c r="E104" s="2">
+        <f t="shared" si="8"/>
+        <v>49.314263580022065</v>
+      </c>
+      <c r="G104" s="1"/>
+      <c r="J104" s="3"/>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A105" s="8">
+        <v>0.999999999999999</v>
+      </c>
+      <c r="B105" s="2">
+        <v>0.412181537273896</v>
+      </c>
+      <c r="C105" s="2">
+        <v>0.32959632737719502</v>
+      </c>
+      <c r="D105" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52775691249855483</v>
+      </c>
+      <c r="E105" s="2">
+        <f t="shared" si="8"/>
+        <v>51.352814920866443</v>
+      </c>
+      <c r="G105" s="1"/>
+      <c r="J105" s="3"/>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A106" s="8">
+        <v>1.00999999999999</v>
+      </c>
+      <c r="B106" s="2">
+        <v>0.42376681117539899</v>
+      </c>
+      <c r="C106" s="2">
+        <v>0.31295065541087302</v>
+      </c>
+      <c r="D106" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52679827541086466</v>
+      </c>
+      <c r="E106" s="2">
+        <f t="shared" si="8"/>
+        <v>53.554231507711577</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A107" s="9">
+        <v>1.01999999999999</v>
+      </c>
+      <c r="B107" s="5">
+        <v>0.433076938550298</v>
+      </c>
+      <c r="C107" s="5">
+        <v>0.29680145878206599</v>
+      </c>
+      <c r="D107" s="5">
+        <f t="shared" si="7"/>
+        <v>0.52502070496244335</v>
+      </c>
+      <c r="E107" s="5">
+        <f t="shared" si="8"/>
+        <v>55.575913833553727</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A108" s="15">
+        <v>1.02999999999999</v>
+      </c>
+      <c r="B108" s="13">
+        <v>0.44467018284260701</v>
+      </c>
+      <c r="C108" s="13">
+        <v>0.280612410199226</v>
+      </c>
+      <c r="D108" s="13">
+        <f t="shared" si="7"/>
+        <v>0.5258088020061058</v>
+      </c>
+      <c r="E108" s="13">
+        <f t="shared" si="8"/>
+        <v>57.745722168944688</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A109" s="8">
+        <v>1.03999999999999</v>
+      </c>
+      <c r="B109" s="2">
+        <v>0.45530235802311397</v>
+      </c>
+      <c r="C109" s="2">
+        <v>0.26169956209710599</v>
+      </c>
+      <c r="D109" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52515416595817355</v>
+      </c>
+      <c r="E109" s="2">
+        <f t="shared" si="8"/>
+        <v>60.110489553279265</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A110" s="8">
+        <v>1.0499999999999901</v>
+      </c>
+      <c r="B110" s="2">
+        <v>0.46867427350451302</v>
+      </c>
+      <c r="C110" s="2">
+        <v>0.242738891650148</v>
+      </c>
+      <c r="D110" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52780464583454112</v>
+      </c>
+      <c r="E110" s="2">
+        <f t="shared" si="8"/>
+        <v>62.619157467256599</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A111" s="8">
+        <v>1.0599999999999901</v>
+      </c>
+      <c r="B111" s="2">
+        <v>0.47882591412911801</v>
+      </c>
+      <c r="C111" s="2">
+        <v>0.222464143788389</v>
+      </c>
+      <c r="D111" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52798158236162607</v>
+      </c>
+      <c r="E111" s="2">
+        <f t="shared" si="8"/>
+        <v>65.08025920033505</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A112" s="15">
+        <v>1.0699999999999901</v>
+      </c>
+      <c r="B112" s="13">
+        <v>0.493511907025319</v>
+      </c>
+      <c r="C112" s="13">
+        <v>0.20028319848463699</v>
+      </c>
+      <c r="D112" s="13">
+        <f t="shared" si="7"/>
+        <v>0.53260432027068993</v>
+      </c>
+      <c r="E112" s="13">
+        <f t="shared" si="8"/>
+        <v>67.911084254465806</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A113" s="8">
+        <v>1.0799999999999901</v>
+      </c>
+      <c r="B113" s="2">
+        <v>0.50637140638759104</v>
+      </c>
+      <c r="C113" s="2">
+        <v>0.17813413474411099</v>
+      </c>
+      <c r="D113" s="2">
+        <f t="shared" si="7"/>
+        <v>0.53679024876387238</v>
+      </c>
+      <c r="E113" s="2">
+        <f t="shared" si="8"/>
+        <v>70.618865624703105</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A114" s="8">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="B114" s="2">
+        <v>0.51693225364837603</v>
+      </c>
+      <c r="C114" s="2">
+        <v>0.15455340382437899</v>
+      </c>
+      <c r="D114" s="2">
+        <f t="shared" si="7"/>
+        <v>0.53954212949100699</v>
+      </c>
+      <c r="E114" s="2">
+        <f t="shared" si="8"/>
+        <v>73.354285436750047</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A115" s="8">
+        <v>1.0999999999999901</v>
+      </c>
+      <c r="B115" s="2">
+        <v>0.52829781670027398</v>
+      </c>
+      <c r="C115" s="2">
+        <v>0.13026333249957001</v>
+      </c>
+      <c r="D115" s="2">
+        <f t="shared" si="7"/>
+        <v>0.54412050037116766</v>
+      </c>
+      <c r="E115" s="2">
+        <f t="shared" si="8"/>
+        <v>76.148773456488229</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A116" s="10">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="B116" s="11">
+        <v>0.54070613466779704</v>
+      </c>
+      <c r="C116" s="11">
+        <v>0.106980237891656</v>
+      </c>
+      <c r="D116" s="11">
+        <f t="shared" si="7"/>
+        <v>0.55118771336700267</v>
+      </c>
+      <c r="E116" s="2">
+        <f t="shared" si="8"/>
+        <v>78.808408424967695</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A117" s="8">
+        <v>1.1199999999999899</v>
+      </c>
+      <c r="B117" s="2">
+        <v>0.552378405985121</v>
+      </c>
+      <c r="C117" s="2">
+        <v>7.0895265130177298E-2</v>
+      </c>
+      <c r="D117" s="2">
+        <f t="shared" si="7"/>
+        <v>0.55690936607004671</v>
+      </c>
+      <c r="E117" s="2">
+        <f t="shared" si="8"/>
+        <v>82.686329745660657</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A118" s="15">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="B118" s="13">
+        <v>0.56266543592266205</v>
+      </c>
+      <c r="C118" s="13">
+        <v>4.3548485455954897E-2</v>
+      </c>
+      <c r="D118" s="2">
+        <f t="shared" si="7"/>
+        <v>0.56434817565714412</v>
+      </c>
+      <c r="E118" s="2">
+        <f t="shared" si="8"/>
+        <v>85.574314850692502</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A119" s="8"/>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A120" s="8"/>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A121" s="8"/>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A122" s="8"/>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A123" s="15"/>
+      <c r="B123" s="13"/>
+      <c r="C123" s="13"/>
+      <c r="D123" s="13"/>
+      <c r="E123" s="13"/>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A124" s="8"/>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A125" s="8"/>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A126" s="8"/>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A127" s="8"/>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A128" s="8"/>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A129" s="8"/>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A130" s="8"/>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A131" s="8"/>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A132" s="8"/>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A133" s="8"/>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A134" s="8"/>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A135" s="8"/>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A136" s="8"/>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A137" s="8"/>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A138" s="8"/>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A139" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
more data for metal track
</commit_message>
<xml_diff>
--- a/Semesteroppgave datasett.xlsx
+++ b/Semesteroppgave datasett.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sondreklyve/semesteroppgave/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0106CEC5-E939-2F4F-A545-3BABF6943DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF93B68C-71E4-9649-9852-92FAB57B6B8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="4" xr2:uid="{0FBCAA18-910F-1F49-A720-95E14FF45760}"/>
   </bookViews>
@@ -17,7 +17,8 @@
     <sheet name="Sylinder filt" sheetId="2" r:id="rId2"/>
     <sheet name="Hul sylinder teip" sheetId="3" r:id="rId3"/>
     <sheet name="Sylinder teip" sheetId="4" r:id="rId4"/>
-    <sheet name="Sylinder metall" sheetId="5" r:id="rId5"/>
+    <sheet name="Hul sylinder metall" sheetId="6" r:id="rId5"/>
+    <sheet name="Sylinder metall" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="16">
   <si>
     <t>t</t>
   </si>
@@ -17283,11 +17284,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B58BE6-65FB-F14F-AB37-8104F299DF65}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AE1A76D-B1D7-0F4F-9E34-A93A595696EC}">
   <dimension ref="A3:Q139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" topLeftCell="E7" workbookViewId="0">
+      <selection activeCell="R28" sqref="R27:R28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17372,6 +17373,4281 @@
         <v>0</v>
       </c>
       <c r="B5" s="2">
+        <v>1.0848123219284101E-2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.52426141224455103</v>
+      </c>
+      <c r="D5" s="2">
+        <f>(B5^2+C5^2)^0.5</f>
+        <v>0.52437363601351261</v>
+      </c>
+      <c r="E5" s="2">
+        <f>DEGREES(ATAN(B5/C5))</f>
+        <v>1.1854066979103586</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.19026293937156499</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0.48581858156100099</v>
+      </c>
+      <c r="J5" s="4">
+        <f>(H5^2+I5^2)^0.5</f>
+        <v>0.52174675877119814</v>
+      </c>
+      <c r="K5" s="2">
+        <f>DEGREES(ATAN(H5/I5))</f>
+        <v>21.386986274949631</v>
+      </c>
+      <c r="M5" s="8">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2">
+        <v>0.35239896196152098</v>
+      </c>
+      <c r="O5" s="2">
+        <v>0.37718675613807001</v>
+      </c>
+      <c r="P5" s="2">
+        <f>(N5^2+O5^2)^0.5</f>
+        <v>0.51619267468409258</v>
+      </c>
+      <c r="Q5" s="2">
+        <f>DEGREES(ATAN(N5/O5))</f>
+        <v>43.054115002980332</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" s="8">
+        <v>9.9999999999997695E-3</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1.0978294512173799E-2</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.52426120086566397</v>
+      </c>
+      <c r="D6" s="2">
+        <f t="shared" ref="D6:D69" si="0">(B6^2+C6^2)^0.5</f>
+        <v>0.52437613378519055</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" ref="E6:E69" si="1">DEGREES(ATAN(B6/C6))</f>
+        <v>1.1996272538521235</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.19046620253090901</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.485721809988927</v>
+      </c>
+      <c r="J6" s="4">
+        <f t="shared" ref="J6:J67" si="2">(H6^2+I6^2)^0.5</f>
+        <v>0.5217308223648135</v>
+      </c>
+      <c r="K6" s="2">
+        <f t="shared" ref="K6:K67" si="3">DEGREES(ATAN(H6/I6))</f>
+        <v>21.411646651112196</v>
+      </c>
+      <c r="M6" s="8">
+        <v>1.0000000000000101E-2</v>
+      </c>
+      <c r="N6" s="2">
+        <v>0.35247212789188098</v>
+      </c>
+      <c r="O6" s="2">
+        <v>0.37719876237691702</v>
+      </c>
+      <c r="P6" s="2">
+        <f t="shared" ref="P6:P41" si="4">(N6^2+O6^2)^0.5</f>
+        <v>0.51625139930009722</v>
+      </c>
+      <c r="Q6" s="2">
+        <f t="shared" ref="Q6:Q35" si="5">DEGREES(ATAN(N6/O6))</f>
+        <v>43.059138871586136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" s="8">
+        <v>1.9999999999999699E-2</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1.11318158491279E-2</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.52426895951639096</v>
+      </c>
+      <c r="D7" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52438712726047931</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="1"/>
+        <v>1.216379934448286</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.19110805543111001</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0.48559808558231099</v>
+      </c>
+      <c r="J7" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52185035170234928</v>
+      </c>
+      <c r="K7" s="2">
+        <f t="shared" si="3"/>
+        <v>21.482213242661128</v>
+      </c>
+      <c r="M7" s="8">
+        <v>2.0000000000000101E-2</v>
+      </c>
+      <c r="N7" s="2">
+        <v>0.35234387484166901</v>
+      </c>
+      <c r="O7" s="2">
+        <v>0.377044803750545</v>
+      </c>
+      <c r="P7" s="2">
+        <f t="shared" si="4"/>
+        <v>0.51605134451305201</v>
+      </c>
+      <c r="Q7" s="2">
+        <f t="shared" si="5"/>
+        <v>43.060405435765979</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="8">
+        <v>2.9999999999999701E-2</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1.1157504693951201E-2</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.52425580750905199</v>
+      </c>
+      <c r="D8" s="2">
+        <f t="shared" si="0"/>
+        <v>0.5243745241885458</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="1"/>
+        <v>1.2192166995484208</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.19196876375144101</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0.485227081032366</v>
+      </c>
+      <c r="J8" s="4">
+        <f t="shared" si="2"/>
+        <v>0.5218211632575348</v>
+      </c>
+      <c r="K8" s="2">
+        <f t="shared" si="3"/>
+        <v>21.585071684361704</v>
+      </c>
+      <c r="M8" s="8">
+        <v>3.00000000000001E-2</v>
+      </c>
+      <c r="N8" s="2">
+        <v>0.35348976278070299</v>
+      </c>
+      <c r="O8" s="2">
+        <v>0.37599350430763201</v>
+      </c>
+      <c r="P8" s="2">
+        <f t="shared" si="4"/>
+        <v>0.51606794869696271</v>
+      </c>
+      <c r="Q8" s="2">
+        <f t="shared" si="5"/>
+        <v>43.233049758144716</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" s="8">
+        <v>3.9999999999999702E-2</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1.11860340382085E-2</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.52430060376006304</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52441991806249177</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="1"/>
+        <v>1.2222288443551879</v>
+      </c>
+      <c r="G9" s="1">
+        <v>4.0000000000000202E-2</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.192662197426333</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0.48505143196761402</v>
+      </c>
+      <c r="J9" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52191341616304154</v>
+      </c>
+      <c r="K9" s="2">
+        <f t="shared" si="3"/>
+        <v>21.662952334066887</v>
+      </c>
+      <c r="M9" s="8">
+        <v>4.0000000000000098E-2</v>
+      </c>
+      <c r="N9" s="2">
+        <v>0.35548798458164899</v>
+      </c>
+      <c r="O9" s="2">
+        <v>0.37442754880408002</v>
+      </c>
+      <c r="P9" s="2">
+        <f t="shared" si="4"/>
+        <v>0.5163019431353657</v>
+      </c>
+      <c r="Q9" s="2">
+        <f t="shared" si="5"/>
+        <v>43.513644926265457</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" s="8">
+        <v>4.9999999999999697E-2</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1.13444876624311E-2</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.52427148651819799</v>
+      </c>
+      <c r="D10" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52439421142526366</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="1"/>
+        <v>1.2396055497611826</v>
+      </c>
+      <c r="G10" s="1">
+        <v>5.0000000000000197E-2</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.19356888538433101</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0.48454754198547101</v>
+      </c>
+      <c r="J10" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52178082930776026</v>
+      </c>
+      <c r="K10" s="2">
+        <f t="shared" si="3"/>
+        <v>21.775907514359545</v>
+      </c>
+      <c r="M10" s="8">
+        <v>5.00000000000001E-2</v>
+      </c>
+      <c r="N10" s="2">
+        <v>0.35660819671358102</v>
+      </c>
+      <c r="O10" s="2">
+        <v>0.37308385038424002</v>
+      </c>
+      <c r="P10" s="2">
+        <f t="shared" si="4"/>
+        <v>0.51610170061804883</v>
+      </c>
+      <c r="Q10" s="2">
+        <f t="shared" si="5"/>
+        <v>43.706543320631184</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" s="8">
+        <v>5.9999999999999699E-2</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1.15488145854567E-2</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.524263892259758</v>
+      </c>
+      <c r="D11" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52439107910573812</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="1"/>
+        <v>1.261943351485552</v>
+      </c>
+      <c r="G11" s="1">
+        <v>6.0000000000000199E-2</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.19490435576764101</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0.48399767241224201</v>
+      </c>
+      <c r="J11" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52176762528703047</v>
+      </c>
+      <c r="K11" s="2">
+        <f t="shared" si="3"/>
+        <v>21.93449256743726</v>
+      </c>
+      <c r="M11" s="8">
+        <v>6.0000000000000102E-2</v>
+      </c>
+      <c r="N11" s="2">
+        <v>0.35851061615824698</v>
+      </c>
+      <c r="O11" s="2">
+        <v>0.37101373292025602</v>
+      </c>
+      <c r="P11" s="2">
+        <f t="shared" si="4"/>
+        <v>0.51592737077382222</v>
+      </c>
+      <c r="Q11" s="2">
+        <f t="shared" si="5"/>
+        <v>44.018119555944693</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" s="8">
+        <v>6.9999999999999701E-2</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1.18270763554847E-2</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.52422231986441603</v>
+      </c>
+      <c r="D12" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52435571931576053</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="1"/>
+        <v>1.2924413818373228</v>
+      </c>
+      <c r="G12" s="1">
+        <v>7.0000000000000201E-2</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0.196356765293596</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0.483415187196301</v>
+      </c>
+      <c r="J12" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52177219405464592</v>
+      </c>
+      <c r="K12" s="2">
+        <f t="shared" si="3"/>
+        <v>22.1063297000231</v>
+      </c>
+      <c r="M12" s="8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="N12" s="2">
+        <v>0.36139294937442001</v>
+      </c>
+      <c r="O12" s="2">
+        <v>0.36822246314361401</v>
+      </c>
+      <c r="P12" s="2">
+        <f t="shared" si="4"/>
+        <v>0.51593860702712713</v>
+      </c>
+      <c r="Q12" s="2">
+        <f t="shared" si="5"/>
+        <v>44.463702547040967</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" s="8">
+        <v>7.9999999999999696E-2</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1.19547345011088E-2</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.52427192933054501</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52440821080620392</v>
+      </c>
+      <c r="E13" s="2">
+        <f t="shared" si="1"/>
+        <v>1.3062632484637993</v>
+      </c>
+      <c r="G13" s="1">
+        <v>8.0000000000000196E-2</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0.19793845355821499</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0.48267407895944903</v>
+      </c>
+      <c r="J13" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52168371442510075</v>
+      </c>
+      <c r="K13" s="2">
+        <f t="shared" si="3"/>
+        <v>22.297905411797082</v>
+      </c>
+      <c r="M13" s="8">
+        <v>0.08</v>
+      </c>
+      <c r="N13" s="2">
+        <v>0.36434699605027299</v>
+      </c>
+      <c r="O13" s="2">
+        <v>0.36522886750932898</v>
+      </c>
+      <c r="P13" s="2">
+        <f t="shared" si="4"/>
+        <v>0.51588841738597369</v>
+      </c>
+      <c r="Q13" s="2">
+        <f t="shared" si="5"/>
+        <v>44.930744024586495</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" s="8">
+        <v>8.9999999999999705E-2</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1.2064456433381001E-2</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.52427608566246897</v>
+      </c>
+      <c r="D14" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52441487879978521</v>
+      </c>
+      <c r="E14" s="2">
+        <f t="shared" si="1"/>
+        <v>1.3182376248662573</v>
+      </c>
+      <c r="G14" s="1">
+        <v>9.0000000000000205E-2</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0.200024047405955</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0.48182320238930998</v>
+      </c>
+      <c r="J14" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52169264696883522</v>
+      </c>
+      <c r="K14" s="2">
+        <f t="shared" si="3"/>
+        <v>22.545288857509568</v>
+      </c>
+      <c r="M14" s="8">
+        <v>0.09</v>
+      </c>
+      <c r="N14" s="2">
+        <v>0.36708143852354203</v>
+      </c>
+      <c r="O14" s="2">
+        <v>0.36184076709149998</v>
+      </c>
+      <c r="P14" s="2">
+        <f t="shared" si="4"/>
+        <v>0.51543915570887522</v>
+      </c>
+      <c r="Q14" s="2">
+        <f t="shared" si="5"/>
+        <v>45.411927609057983</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" s="8">
+        <v>9.99999999999997E-2</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1.24119667467771E-2</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.52426403400880295</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="0"/>
+        <v>0.5244109402688949</v>
+      </c>
+      <c r="E15" s="2">
+        <f t="shared" si="1"/>
+        <v>1.3562259468054778</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0.202412136335893</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0.48094824631676802</v>
+      </c>
+      <c r="J15" s="4">
+        <f t="shared" si="2"/>
+        <v>0.5218063707652818</v>
+      </c>
+      <c r="K15" s="2">
+        <f t="shared" si="3"/>
+        <v>22.824304643692564</v>
+      </c>
+      <c r="M15" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="N15" s="2">
+        <v>0.37091322060910398</v>
+      </c>
+      <c r="O15" s="2">
+        <v>0.35796917130640798</v>
+      </c>
+      <c r="P15" s="2">
+        <f t="shared" si="4"/>
+        <v>0.5154789470273391</v>
+      </c>
+      <c r="Q15" s="2">
+        <f t="shared" si="5"/>
+        <v>46.017395197526504</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16" s="8">
+        <v>0.109999999999999</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1.28535060421738E-2</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.52421812929006895</v>
+      </c>
+      <c r="D16" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52437568564337111</v>
+      </c>
+      <c r="E16" s="2">
+        <f t="shared" si="1"/>
+        <v>1.404575834503071</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0.20508896367412299</v>
+      </c>
+      <c r="I16" s="2">
+        <v>0.47979766330407603</v>
+      </c>
+      <c r="J16" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52179237320315175</v>
+      </c>
+      <c r="K16" s="2">
+        <f t="shared" si="3"/>
+        <v>23.144230387785239</v>
+      </c>
+      <c r="M16" s="8">
+        <v>0.11</v>
+      </c>
+      <c r="N16" s="2">
+        <v>0.37481134034319802</v>
+      </c>
+      <c r="O16" s="2">
+        <v>0.353756147710308</v>
+      </c>
+      <c r="P16" s="2">
+        <f t="shared" si="4"/>
+        <v>0.51539009778293365</v>
+      </c>
+      <c r="Q16" s="2">
+        <f t="shared" si="5"/>
+        <v>46.655355224087842</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A17" s="8">
+        <v>0.119999999999999</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1.30248443573592E-2</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.52418242946420801</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52434422465545738</v>
+      </c>
+      <c r="E17" s="2">
+        <f t="shared" si="1"/>
+        <v>1.4233881918874989</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0.20786915389372199</v>
+      </c>
+      <c r="I17" s="2">
+        <v>0.478638771997838</v>
+      </c>
+      <c r="J17" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52182818934979958</v>
+      </c>
+      <c r="K17" s="2">
+        <f t="shared" si="3"/>
+        <v>23.474937144946527</v>
+      </c>
+      <c r="M17" s="8">
+        <v>0.12</v>
+      </c>
+      <c r="N17" s="2">
+        <v>0.378425396156506</v>
+      </c>
+      <c r="O17" s="2">
+        <v>0.349287262239042</v>
+      </c>
+      <c r="P17" s="2">
+        <f t="shared" si="4"/>
+        <v>0.51498288517061785</v>
+      </c>
+      <c r="Q17" s="2">
+        <f t="shared" si="5"/>
+        <v>47.292939012584647</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A18" s="8">
+        <v>0.12999999999999901</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1.33009626700133E-2</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.52421024622023704</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="shared" si="0"/>
+        <v>0.5243789639661669</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="shared" si="1"/>
+        <v>1.4534731955722224</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0.13</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0.21111446511155901</v>
+      </c>
+      <c r="I18" s="2">
+        <v>0.477518411313687</v>
+      </c>
+      <c r="J18" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52210453984129201</v>
+      </c>
+      <c r="K18" s="2">
+        <f t="shared" si="3"/>
+        <v>23.850580521182454</v>
+      </c>
+      <c r="M18" s="8">
+        <v>0.13</v>
+      </c>
+      <c r="N18" s="2">
+        <v>0.38309067155744903</v>
+      </c>
+      <c r="O18" s="2">
+        <v>0.34487491340535398</v>
+      </c>
+      <c r="P18" s="2">
+        <f t="shared" si="4"/>
+        <v>0.51545821220607957</v>
+      </c>
+      <c r="Q18" s="2">
+        <f t="shared" si="5"/>
+        <v>48.005078231004262</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A19" s="8">
+        <v>0.13999999999999899</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1.36920971041432E-2</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.52418993010043702</v>
+      </c>
+      <c r="D19" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52436872174244942</v>
+      </c>
+      <c r="E19" s="2">
+        <f t="shared" si="1"/>
+        <v>1.4962535307456564</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0.214088915978699</v>
+      </c>
+      <c r="I19" s="2">
+        <v>0.47630688002084698</v>
+      </c>
+      <c r="J19" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52220906531783606</v>
+      </c>
+      <c r="K19" s="2">
+        <f t="shared" si="3"/>
+        <v>24.202813787913364</v>
+      </c>
+      <c r="M19" s="8">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="N19" s="2">
+        <v>0.38795113089225203</v>
+      </c>
+      <c r="O19" s="2">
+        <v>0.33892442986849303</v>
+      </c>
+      <c r="P19" s="2">
+        <f t="shared" si="4"/>
+        <v>0.5151464346399578</v>
+      </c>
+      <c r="Q19" s="2">
+        <f t="shared" si="5"/>
+        <v>48.858672778002905</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A20" s="8">
+        <v>0.149999999999999</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1.39108461559759E-2</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.52411680634714997</v>
+      </c>
+      <c r="D20" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52430138120770875</v>
+      </c>
+      <c r="E20" s="2">
+        <f t="shared" si="1"/>
+        <v>1.5203589862161278</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="H20" s="2">
+        <v>0.217922003199846</v>
+      </c>
+      <c r="I20" s="2">
+        <v>0.47447708870105598</v>
+      </c>
+      <c r="J20" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52212882240005043</v>
+      </c>
+      <c r="K20" s="2">
+        <f t="shared" si="3"/>
+        <v>24.668788013369589</v>
+      </c>
+      <c r="M20" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="N20" s="2">
+        <v>0.39365649747934101</v>
+      </c>
+      <c r="O20" s="2">
+        <v>0.33191808396885902</v>
+      </c>
+      <c r="P20" s="2">
+        <f t="shared" si="4"/>
+        <v>0.51491266489887488</v>
+      </c>
+      <c r="Q20" s="2">
+        <f t="shared" si="5"/>
+        <v>49.863525466287626</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A21" s="8">
+        <v>0.159999999999999</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1.44443514199493E-2</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.52408749270833099</v>
+      </c>
+      <c r="D21" s="2">
+        <f t="shared" si="0"/>
+        <v>0.5242865049772385</v>
+      </c>
+      <c r="E21" s="2">
+        <f t="shared" si="1"/>
+        <v>1.5787267030921648</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0.16</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0.22206959383955499</v>
+      </c>
+      <c r="I21" s="2">
+        <v>0.47251902802870599</v>
+      </c>
+      <c r="J21" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52210069561077765</v>
+      </c>
+      <c r="K21" s="2">
+        <f t="shared" si="3"/>
+        <v>25.172099376239224</v>
+      </c>
+      <c r="M21" s="15">
+        <v>0.16</v>
+      </c>
+      <c r="N21" s="13">
+        <v>0.39865187124711599</v>
+      </c>
+      <c r="O21" s="13">
+        <v>0.32568070705344798</v>
+      </c>
+      <c r="P21" s="13">
+        <f t="shared" si="4"/>
+        <v>0.51477299598527981</v>
+      </c>
+      <c r="Q21" s="2">
+        <f t="shared" si="5"/>
+        <v>50.752717943364495</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A22" s="8">
+        <v>0.16999999999999901</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1.4893748879561399E-2</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.52406692980504599</v>
+      </c>
+      <c r="D22" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52427852394597896</v>
+      </c>
+      <c r="E22" s="2">
+        <f t="shared" si="1"/>
+        <v>1.6278823808838301</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0.17</v>
+      </c>
+      <c r="H22" s="2">
+        <v>0.22584932659020701</v>
+      </c>
+      <c r="I22" s="2">
+        <v>0.470472284732533</v>
+      </c>
+      <c r="J22" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52187363319361091</v>
+      </c>
+      <c r="K22" s="2">
+        <f t="shared" si="3"/>
+        <v>25.643245664879466</v>
+      </c>
+      <c r="M22" s="8">
+        <v>0.17</v>
+      </c>
+      <c r="N22" s="2">
+        <v>0.40439363528790501</v>
+      </c>
+      <c r="O22" s="2">
+        <v>0.31858235616904901</v>
+      </c>
+      <c r="P22" s="2">
+        <f t="shared" si="4"/>
+        <v>0.51480960550827914</v>
+      </c>
+      <c r="Q22" s="2">
+        <f t="shared" si="5"/>
+        <v>51.768868364587675</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A23" s="8">
+        <v>0.18</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1.5449296734963199E-2</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.524096181416423</v>
+      </c>
+      <c r="D23" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52432383900112833</v>
+      </c>
+      <c r="E23" s="2">
+        <f t="shared" si="1"/>
+        <v>1.688474886295432</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0.18</v>
+      </c>
+      <c r="H23" s="2">
+        <v>0.22993838166296299</v>
+      </c>
+      <c r="I23" s="2">
+        <v>0.46819279940252101</v>
+      </c>
+      <c r="J23" s="4">
+        <f t="shared" si="2"/>
+        <v>0.5216091992806029</v>
+      </c>
+      <c r="K23" s="2">
+        <f t="shared" si="3"/>
+        <v>26.156532014941725</v>
+      </c>
+      <c r="M23" s="8">
+        <v>0.18</v>
+      </c>
+      <c r="N23" s="2">
+        <v>0.41072669678552398</v>
+      </c>
+      <c r="O23" s="2">
+        <v>0.30984281435331201</v>
+      </c>
+      <c r="P23" s="2">
+        <f t="shared" si="4"/>
+        <v>0.51448905630608777</v>
+      </c>
+      <c r="Q23" s="2">
+        <f t="shared" si="5"/>
+        <v>52.969934104236735</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A24" s="8">
+        <v>0.19</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1.5972828954662399E-2</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.52408630792211797</v>
+      </c>
+      <c r="D24" s="2">
+        <f t="shared" si="0"/>
+        <v>0.5243296571969317</v>
+      </c>
+      <c r="E24" s="2">
+        <f t="shared" si="1"/>
+        <v>1.7456904868456304</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0.19</v>
+      </c>
+      <c r="H24" s="2">
+        <v>0.23461341429034299</v>
+      </c>
+      <c r="I24" s="2">
+        <v>0.46551656673809899</v>
+      </c>
+      <c r="J24" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52129562445180666</v>
+      </c>
+      <c r="K24" s="2">
+        <f t="shared" si="3"/>
+        <v>26.747423463901718</v>
+      </c>
+      <c r="M24" s="8">
+        <v>0.19</v>
+      </c>
+      <c r="N24" s="2">
+        <v>0.41680581576190501</v>
+      </c>
+      <c r="O24" s="2">
+        <v>0.30209972054273099</v>
+      </c>
+      <c r="P24" s="2">
+        <f t="shared" si="4"/>
+        <v>0.51477308515980447</v>
+      </c>
+      <c r="Q24" s="2">
+        <f t="shared" si="5"/>
+        <v>54.06550222659164</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A25" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="B25" s="2">
+        <v>1.6405298405951299E-2</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.52394760175643895</v>
+      </c>
+      <c r="D25" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52420437159767397</v>
+      </c>
+      <c r="E25" s="2">
+        <f t="shared" si="1"/>
+        <v>1.7933995083453895</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0.239107625378779</v>
+      </c>
+      <c r="I25" s="2">
+        <v>0.46302186361178199</v>
+      </c>
+      <c r="J25" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52111582464631234</v>
+      </c>
+      <c r="K25" s="2">
+        <f t="shared" si="3"/>
+        <v>27.312136629020351</v>
+      </c>
+      <c r="M25" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="N25" s="2">
+        <v>0.42768983072254801</v>
+      </c>
+      <c r="O25" s="2">
+        <v>0.29066250841504998</v>
+      </c>
+      <c r="P25" s="2">
+        <f t="shared" si="4"/>
+        <v>0.51711051536553654</v>
+      </c>
+      <c r="Q25" s="2">
+        <f t="shared" si="5"/>
+        <v>55.799560162788396</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A26" s="8">
+        <v>0.21</v>
+      </c>
+      <c r="B26" s="2">
+        <v>1.7001995222546199E-2</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.52397982731970905</v>
+      </c>
+      <c r="D26" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52425559346519102</v>
+      </c>
+      <c r="E26" s="2">
+        <f t="shared" si="1"/>
+        <v>1.8584702234554091</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0.24387229494455601</v>
+      </c>
+      <c r="I26" s="2">
+        <v>0.45991940153233002</v>
+      </c>
+      <c r="J26" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52057617324209249</v>
+      </c>
+      <c r="K26" s="2">
+        <f t="shared" si="3"/>
+        <v>27.934774416469324</v>
+      </c>
+      <c r="M26" s="8">
+        <v>0.21</v>
+      </c>
+      <c r="N26" s="2">
+        <v>0.43436174261538002</v>
+      </c>
+      <c r="O26" s="2">
+        <v>0.28109900788373299</v>
+      </c>
+      <c r="P26" s="2">
+        <f t="shared" si="4"/>
+        <v>0.51738455299814334</v>
+      </c>
+      <c r="Q26" s="2">
+        <f t="shared" si="5"/>
+        <v>57.090907008390587</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A27" s="8">
+        <v>0.22</v>
+      </c>
+      <c r="B27" s="2">
+        <v>1.7606545995929802E-2</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.523905331517458</v>
+      </c>
+      <c r="D27" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52420109390798142</v>
+      </c>
+      <c r="E27" s="2">
+        <f t="shared" si="1"/>
+        <v>1.9247776381608168</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0.22</v>
+      </c>
+      <c r="H27" s="2">
+        <v>0.24884786246737201</v>
+      </c>
+      <c r="I27" s="2">
+        <v>0.456016381753862</v>
+      </c>
+      <c r="J27" s="4">
+        <f t="shared" si="2"/>
+        <v>0.51949610112344835</v>
+      </c>
+      <c r="K27" s="2">
+        <f t="shared" si="3"/>
+        <v>28.621270480414783</v>
+      </c>
+      <c r="M27" s="15">
+        <v>0.22</v>
+      </c>
+      <c r="N27" s="13">
+        <v>0.441434413911173</v>
+      </c>
+      <c r="O27" s="13">
+        <v>0.26996264179160401</v>
+      </c>
+      <c r="P27" s="13">
+        <f t="shared" si="4"/>
+        <v>0.51744001560393715</v>
+      </c>
+      <c r="Q27" s="13">
+        <f t="shared" si="5"/>
+        <v>58.551805428692333</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A28" s="8">
+        <v>0.23</v>
+      </c>
+      <c r="B28" s="2">
+        <v>1.83787341920265E-2</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0.52383987319298597</v>
+      </c>
+      <c r="D28" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52416217968997414</v>
+      </c>
+      <c r="E28" s="2">
+        <f t="shared" si="1"/>
+        <v>2.0093776891045616</v>
+      </c>
+      <c r="G28" s="1">
+        <v>0.23</v>
+      </c>
+      <c r="H28" s="2">
+        <v>0.25396998024692602</v>
+      </c>
+      <c r="I28" s="2">
+        <v>0.45255625053217302</v>
+      </c>
+      <c r="J28" s="4">
+        <f t="shared" si="2"/>
+        <v>0.51894885177863426</v>
+      </c>
+      <c r="K28" s="2">
+        <f t="shared" si="3"/>
+        <v>29.300698707964116</v>
+      </c>
+      <c r="M28" s="15">
+        <v>0.23</v>
+      </c>
+      <c r="N28" s="13">
+        <v>0.44879012503589999</v>
+      </c>
+      <c r="O28" s="13">
+        <v>0.25845748865887003</v>
+      </c>
+      <c r="P28" s="13">
+        <f t="shared" si="4"/>
+        <v>0.51789270102366636</v>
+      </c>
+      <c r="Q28" s="13">
+        <f t="shared" si="5"/>
+        <v>60.062431225553638</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A29" s="8">
+        <v>0.24</v>
+      </c>
+      <c r="B29" s="2">
+        <v>1.90025911245435E-2</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0.52384995045538196</v>
+      </c>
+      <c r="D29" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52419449545140473</v>
+      </c>
+      <c r="E29" s="2">
+        <f t="shared" si="1"/>
+        <v>2.0774862898992059</v>
+      </c>
+      <c r="G29" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="H29" s="2">
+        <v>0.25923611456817502</v>
+      </c>
+      <c r="I29" s="2">
+        <v>0.44890242765233301</v>
+      </c>
+      <c r="J29" s="4">
+        <f t="shared" si="2"/>
+        <v>0.51837896624820923</v>
+      </c>
+      <c r="K29" s="2">
+        <f t="shared" si="3"/>
+        <v>30.005951638138335</v>
+      </c>
+      <c r="M29" s="15">
+        <v>0.24</v>
+      </c>
+      <c r="N29" s="13">
+        <v>0.45621692555291699</v>
+      </c>
+      <c r="O29" s="13">
+        <v>0.24690830463004501</v>
+      </c>
+      <c r="P29" s="13">
+        <f t="shared" si="4"/>
+        <v>0.51874617497986319</v>
+      </c>
+      <c r="Q29" s="13">
+        <f t="shared" si="5"/>
+        <v>61.577388193718861</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A30" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="B30" s="2">
+        <v>1.9620749234779501E-2</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0.52390653022865596</v>
+      </c>
+      <c r="D30" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52427380844055493</v>
+      </c>
+      <c r="E30" s="2">
+        <f t="shared" si="1"/>
+        <v>2.1447737659674369</v>
+      </c>
+      <c r="G30" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="H30" s="2">
+        <v>0.26448317752601502</v>
+      </c>
+      <c r="I30" s="2">
+        <v>0.44475907058932601</v>
+      </c>
+      <c r="J30" s="4">
+        <f t="shared" si="2"/>
+        <v>0.51745722728138477</v>
+      </c>
+      <c r="K30" s="2">
+        <f t="shared" si="3"/>
+        <v>30.738517833375003</v>
+      </c>
+      <c r="M30" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="N30" s="5">
+        <v>0.46479526177316899</v>
+      </c>
+      <c r="O30" s="5">
+        <v>0.23340320710260501</v>
+      </c>
+      <c r="P30" s="5">
+        <f t="shared" si="4"/>
+        <v>0.52010738550088886</v>
+      </c>
+      <c r="Q30" s="5">
+        <f t="shared" si="5"/>
+        <v>63.335867952222941</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A31" s="8">
+        <v>0.26</v>
+      </c>
+      <c r="B31" s="2">
+        <v>2.0165259619607901E-2</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0.52393477909946096</v>
+      </c>
+      <c r="D31" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52432269686284527</v>
+      </c>
+      <c r="E31" s="2">
+        <f t="shared" si="1"/>
+        <v>2.2041183712241681</v>
+      </c>
+      <c r="G31" s="1">
+        <v>0.26</v>
+      </c>
+      <c r="H31" s="2">
+        <v>0.26970439660453499</v>
+      </c>
+      <c r="I31" s="2">
+        <v>0.44066904755944097</v>
+      </c>
+      <c r="J31" s="4">
+        <f t="shared" si="2"/>
+        <v>0.51665236961109662</v>
+      </c>
+      <c r="K31" s="2">
+        <f t="shared" si="3"/>
+        <v>31.468045389098748</v>
+      </c>
+      <c r="M31" s="15">
+        <v>0.26</v>
+      </c>
+      <c r="N31" s="13">
+        <v>0.47238865508623401</v>
+      </c>
+      <c r="O31" s="13">
+        <v>0.22074193226925501</v>
+      </c>
+      <c r="P31" s="13">
+        <f t="shared" si="4"/>
+        <v>0.52141925752329599</v>
+      </c>
+      <c r="Q31" s="13">
+        <f t="shared" si="5"/>
+        <v>64.953842019595029</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A32" s="8">
+        <v>0.26999999999999902</v>
+      </c>
+      <c r="B32" s="2">
+        <v>2.0923889257420801E-2</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0.52395606441175302</v>
+      </c>
+      <c r="D32" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52437368982006516</v>
+      </c>
+      <c r="E32" s="2">
+        <f t="shared" si="1"/>
+        <v>2.2868594207437334</v>
+      </c>
+      <c r="G32" s="1">
+        <v>0.27</v>
+      </c>
+      <c r="H32" s="2">
+        <v>0.27435008309326903</v>
+      </c>
+      <c r="I32" s="2">
+        <v>0.43647214451557098</v>
+      </c>
+      <c r="J32" s="4">
+        <f t="shared" si="2"/>
+        <v>0.51553457792014801</v>
+      </c>
+      <c r="K32" s="2">
+        <f t="shared" si="3"/>
+        <v>32.151934166986713</v>
+      </c>
+      <c r="M32" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="N32" s="2">
+        <v>0.47911465007299597</v>
+      </c>
+      <c r="O32" s="2">
+        <v>0.20416926969730401</v>
+      </c>
+      <c r="P32" s="2">
+        <f t="shared" si="4"/>
+        <v>0.52080316685221861</v>
+      </c>
+      <c r="Q32" s="2">
+        <f t="shared" si="5"/>
+        <v>66.919271966834131</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A33" s="8">
+        <v>0.27999999999999903</v>
+      </c>
+      <c r="B33" s="2">
+        <v>2.1628686418345301E-2</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0.52388220848994504</v>
+      </c>
+      <c r="D33" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52432849288254912</v>
+      </c>
+      <c r="E33" s="2">
+        <f t="shared" si="1"/>
+        <v>2.364136562072491</v>
+      </c>
+      <c r="G33" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H33" s="2">
+        <v>0.28173783105394601</v>
+      </c>
+      <c r="I33" s="2">
+        <v>0.43759338164205203</v>
+      </c>
+      <c r="J33" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52044612891624853</v>
+      </c>
+      <c r="K33" s="2">
+        <f t="shared" si="3"/>
+        <v>32.774842745639418</v>
+      </c>
+      <c r="M33" s="8">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="N33" s="2">
+        <v>0.48635774761540901</v>
+      </c>
+      <c r="O33" s="2">
+        <v>0.18816780275397699</v>
+      </c>
+      <c r="P33" s="2">
+        <f t="shared" si="4"/>
+        <v>0.52148919515057401</v>
+      </c>
+      <c r="Q33" s="2">
+        <f t="shared" si="5"/>
+        <v>68.848956803888328</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A34" s="8">
+        <v>0.28999999999999898</v>
+      </c>
+      <c r="B34" s="2">
+        <v>2.2321515842526701E-2</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0.524005591919952</v>
+      </c>
+      <c r="D34" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52448080082390758</v>
+      </c>
+      <c r="E34" s="2">
+        <f t="shared" si="1"/>
+        <v>2.4392028238440089</v>
+      </c>
+      <c r="G34" s="1">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H34" s="2">
+        <v>0.28746445624753397</v>
+      </c>
+      <c r="I34" s="2">
+        <v>0.432662511829216</v>
+      </c>
+      <c r="J34" s="4">
+        <f t="shared" si="2"/>
+        <v>0.51945419696837258</v>
+      </c>
+      <c r="K34" s="2">
+        <f t="shared" si="3"/>
+        <v>33.600383164104983</v>
+      </c>
+      <c r="M34" s="8">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="N34" s="2">
+        <v>0.49380652564093802</v>
+      </c>
+      <c r="O34" s="2">
+        <v>0.170422993936062</v>
+      </c>
+      <c r="P34" s="2">
+        <f t="shared" si="4"/>
+        <v>0.52238767369426453</v>
+      </c>
+      <c r="Q34" s="2">
+        <f t="shared" si="5"/>
+        <v>70.959371321932323</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A35" s="8">
+        <v>0.29999999999999899</v>
+      </c>
+      <c r="B35" s="2">
+        <v>2.3083565965517298E-2</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0.52396017978373399</v>
+      </c>
+      <c r="D35" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52446841755885287</v>
+      </c>
+      <c r="E35" s="2">
+        <f t="shared" si="1"/>
+        <v>2.52258905895517</v>
+      </c>
+      <c r="G35" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="H35" s="2">
+        <v>0.29355596079833701</v>
+      </c>
+      <c r="I35" s="2">
+        <v>0.42778348098241198</v>
+      </c>
+      <c r="J35" s="4">
+        <f t="shared" si="2"/>
+        <v>0.51881963023931965</v>
+      </c>
+      <c r="K35" s="2">
+        <f t="shared" si="3"/>
+        <v>34.458909768955515</v>
+      </c>
+      <c r="M35" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="N35" s="2">
+        <v>0.50132973395346903</v>
+      </c>
+      <c r="O35" s="2">
+        <v>0.15171112616744101</v>
+      </c>
+      <c r="P35" s="2">
+        <f t="shared" si="4"/>
+        <v>0.52378217605112265</v>
+      </c>
+      <c r="Q35" s="2">
+        <f t="shared" si="5"/>
+        <v>73.163268936314324</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A36" s="8">
+        <v>0.309999999999999</v>
+      </c>
+      <c r="B36" s="2">
+        <v>2.3807926438275E-2</v>
+      </c>
+      <c r="C36" s="2">
+        <v>0.52382866777478898</v>
+      </c>
+      <c r="D36" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52436942182396618</v>
+      </c>
+      <c r="E36" s="2">
+        <f t="shared" si="1"/>
+        <v>2.6022928609782685</v>
+      </c>
+      <c r="G36" s="1">
+        <v>0.31</v>
+      </c>
+      <c r="H36" s="2">
+        <v>0.30011391483045702</v>
+      </c>
+      <c r="I36" s="2">
+        <v>0.42226126424795302</v>
+      </c>
+      <c r="J36" s="4">
+        <f t="shared" si="2"/>
+        <v>0.51804723448653056</v>
+      </c>
+      <c r="K36" s="2">
+        <f t="shared" si="3"/>
+        <v>35.402565209477473</v>
+      </c>
+      <c r="M36" s="8">
+        <v>0.31</v>
+      </c>
+      <c r="N36" s="2">
+        <v>0.50873229756946903</v>
+      </c>
+      <c r="O36" s="2">
+        <v>0.13292581144886301</v>
+      </c>
+      <c r="P36" s="2">
+        <f t="shared" si="4"/>
+        <v>0.52581158406757211</v>
+      </c>
+      <c r="Q36" s="2">
+        <f>DEGREES(ATAN(N36/O36))</f>
+        <v>75.356663747302917</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A37" s="8">
+        <v>0.31999999999999901</v>
+      </c>
+      <c r="B37" s="2">
+        <v>2.47678014060621E-2</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0.52384039329127696</v>
+      </c>
+      <c r="D37" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52442559208151718</v>
+      </c>
+      <c r="E37" s="2">
+        <f t="shared" si="1"/>
+        <v>2.7069971277689353</v>
+      </c>
+      <c r="G37" s="1">
+        <v>0.32</v>
+      </c>
+      <c r="H37" s="2">
+        <v>0.30739934802048602</v>
+      </c>
+      <c r="I37" s="2">
+        <v>0.41626203955778102</v>
+      </c>
+      <c r="J37" s="4">
+        <f t="shared" si="2"/>
+        <v>0.51746347188977848</v>
+      </c>
+      <c r="K37" s="2">
+        <f t="shared" si="3"/>
+        <v>36.444962095131856</v>
+      </c>
+      <c r="M37" s="8">
+        <v>0.32</v>
+      </c>
+      <c r="N37" s="2">
+        <v>0.51623996212736301</v>
+      </c>
+      <c r="O37" s="2">
+        <v>0.11217357875251199</v>
+      </c>
+      <c r="P37" s="2">
+        <f t="shared" si="4"/>
+        <v>0.52828648503194475</v>
+      </c>
+      <c r="Q37" s="2">
+        <f t="shared" ref="Q37:Q41" si="6">DEGREES(ATAN(N37/O37))</f>
+        <v>77.740790246831494</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A38" s="8">
+        <v>0.32999999999999902</v>
+      </c>
+      <c r="B38" s="2">
+        <v>2.56933138894039E-2</v>
+      </c>
+      <c r="C38" s="2">
+        <v>0.52383143661970999</v>
+      </c>
+      <c r="D38" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52446117146047011</v>
+      </c>
+      <c r="E38" s="2">
+        <f t="shared" si="1"/>
+        <v>2.8080399753258556</v>
+      </c>
+      <c r="G38" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="H38" s="2">
+        <v>0.31319264311661099</v>
+      </c>
+      <c r="I38" s="2">
+        <v>0.41299131057711802</v>
+      </c>
+      <c r="J38" s="4">
+        <f t="shared" si="2"/>
+        <v>0.51831597921979444</v>
+      </c>
+      <c r="K38" s="2">
+        <f t="shared" si="3"/>
+        <v>37.174921241957222</v>
+      </c>
+      <c r="M38" s="8">
+        <v>0.33</v>
+      </c>
+      <c r="N38" s="2">
+        <v>0.52369606042077199</v>
+      </c>
+      <c r="O38" s="2">
+        <v>9.0541062620379906E-2</v>
+      </c>
+      <c r="P38" s="2">
+        <f t="shared" si="4"/>
+        <v>0.5314651895662259</v>
+      </c>
+      <c r="Q38" s="2">
+        <f t="shared" si="6"/>
+        <v>80.191177695678419</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A39" s="8">
+        <v>0.33999999999999903</v>
+      </c>
+      <c r="B39" s="2">
+        <v>2.6702250236449E-2</v>
+      </c>
+      <c r="C39" s="2">
+        <v>0.52382773322694398</v>
+      </c>
+      <c r="D39" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52450786864008847</v>
+      </c>
+      <c r="E39" s="2">
+        <f t="shared" si="1"/>
+        <v>2.9181409236484579</v>
+      </c>
+      <c r="G39" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="H39" s="2">
+        <v>0.31908898097870703</v>
+      </c>
+      <c r="I39" s="2">
+        <v>0.408644187253556</v>
+      </c>
+      <c r="J39" s="4">
+        <f t="shared" si="2"/>
+        <v>0.518466825899352</v>
+      </c>
+      <c r="K39" s="2">
+        <f t="shared" si="3"/>
+        <v>37.984425287857306</v>
+      </c>
+      <c r="M39" s="8">
+        <v>0.34</v>
+      </c>
+      <c r="N39" s="2">
+        <v>0.53340438244045396</v>
+      </c>
+      <c r="O39" s="2">
+        <v>5.2247272577507498E-2</v>
+      </c>
+      <c r="P39" s="2">
+        <f t="shared" si="4"/>
+        <v>0.53595709968100103</v>
+      </c>
+      <c r="Q39" s="2">
+        <f t="shared" si="6"/>
+        <v>84.405690390214346</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A40" s="8">
+        <v>0.34999999999999898</v>
+      </c>
+      <c r="B40" s="2">
+        <v>2.7737642738443501E-2</v>
+      </c>
+      <c r="C40" s="2">
+        <v>0.523808655808218</v>
+      </c>
+      <c r="D40" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52454254805906619</v>
+      </c>
+      <c r="E40" s="2">
+        <f t="shared" si="1"/>
+        <v>3.0311963471074108</v>
+      </c>
+      <c r="G40" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="H40" s="2">
+        <v>0.32683931270855299</v>
+      </c>
+      <c r="I40" s="2">
+        <v>0.40307672328674898</v>
+      </c>
+      <c r="J40" s="4">
+        <f t="shared" si="2"/>
+        <v>0.51893620146158781</v>
+      </c>
+      <c r="K40" s="2">
+        <f t="shared" si="3"/>
+        <v>39.037257966683406</v>
+      </c>
+      <c r="M40" s="8">
+        <v>0.35</v>
+      </c>
+      <c r="N40" s="2">
+        <v>0.54027901133105705</v>
+      </c>
+      <c r="O40" s="2">
+        <v>2.85823958111515E-2</v>
+      </c>
+      <c r="P40" s="2">
+        <f t="shared" si="4"/>
+        <v>0.54103453072347407</v>
+      </c>
+      <c r="Q40" s="2">
+        <f t="shared" si="6"/>
+        <v>86.971702780335306</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A41" s="8">
+        <v>0.35999999999999899</v>
+      </c>
+      <c r="B41" s="2">
+        <v>2.8817072708510999E-2</v>
+      </c>
+      <c r="C41" s="2">
+        <v>0.52386082444892301</v>
+      </c>
+      <c r="D41" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52465282527762391</v>
+      </c>
+      <c r="E41" s="2">
+        <f t="shared" si="1"/>
+        <v>3.1486115818712235</v>
+      </c>
+      <c r="G41" s="1">
+        <v>0.36</v>
+      </c>
+      <c r="H41" s="2">
+        <v>0.33473037174363202</v>
+      </c>
+      <c r="I41" s="2">
+        <v>0.39760933244157698</v>
+      </c>
+      <c r="J41" s="4">
+        <f t="shared" si="2"/>
+        <v>0.51974763396504897</v>
+      </c>
+      <c r="K41" s="2">
+        <f t="shared" si="3"/>
+        <v>40.092598469908694</v>
+      </c>
+      <c r="M41" s="8">
+        <v>0.36</v>
+      </c>
+      <c r="N41" s="2">
+        <v>0.54709608929774101</v>
+      </c>
+      <c r="O41" s="2">
+        <v>1.0012314809858799E-2</v>
+      </c>
+      <c r="P41" s="2">
+        <f t="shared" si="4"/>
+        <v>0.54718769848447202</v>
+      </c>
+      <c r="Q41" s="2">
+        <f t="shared" si="6"/>
+        <v>88.95155647798066</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A42" s="8">
+        <v>0.369999999999999</v>
+      </c>
+      <c r="B42" s="2">
+        <v>2.99719975856759E-2</v>
+      </c>
+      <c r="C42" s="2">
+        <v>0.52381788288953202</v>
+      </c>
+      <c r="D42" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52467465640542166</v>
+      </c>
+      <c r="E42" s="2">
+        <f t="shared" si="1"/>
+        <v>3.2747995352003878</v>
+      </c>
+      <c r="G42" s="1">
+        <v>0.37</v>
+      </c>
+      <c r="H42" s="2">
+        <v>0.34329808497058401</v>
+      </c>
+      <c r="I42" s="2">
+        <v>0.39135808782794701</v>
+      </c>
+      <c r="J42" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52059074910414749</v>
+      </c>
+      <c r="K42" s="2">
+        <f t="shared" si="3"/>
+        <v>41.257137193037181</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A43" s="8">
+        <v>0.37999999999999901</v>
+      </c>
+      <c r="B43" s="2">
+        <v>3.1059045751643401E-2</v>
+      </c>
+      <c r="C43" s="2">
+        <v>0.52385785644798899</v>
+      </c>
+      <c r="D43" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52477777971755291</v>
+      </c>
+      <c r="E43" s="2">
+        <f t="shared" si="1"/>
+        <v>3.3930415381326626</v>
+      </c>
+      <c r="G43" s="1">
+        <v>0.38</v>
+      </c>
+      <c r="H43" s="2">
+        <v>0.35189733568597098</v>
+      </c>
+      <c r="I43" s="2">
+        <v>0.38476358419750001</v>
+      </c>
+      <c r="J43" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52141610119691517</v>
+      </c>
+      <c r="K43" s="2">
+        <f t="shared" si="3"/>
+        <v>42.44543340872287</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A44" s="8">
+        <v>0.38999999999999901</v>
+      </c>
+      <c r="B44" s="2">
+        <v>3.2298912057790098E-2</v>
+      </c>
+      <c r="C44" s="2">
+        <v>0.52396598440525499</v>
+      </c>
+      <c r="D44" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52496054378770673</v>
+      </c>
+      <c r="E44" s="2">
+        <f t="shared" si="1"/>
+        <v>3.5274287294577431</v>
+      </c>
+      <c r="G44" s="1">
+        <v>0.39</v>
+      </c>
+      <c r="H44" s="2">
+        <v>0.36033535103432601</v>
+      </c>
+      <c r="I44" s="2">
+        <v>0.37710516401497901</v>
+      </c>
+      <c r="J44" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52158400083955325</v>
+      </c>
+      <c r="K44" s="2">
+        <f t="shared" si="3"/>
+        <v>43.697286206230487</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A45" s="8">
+        <v>0.39999999999999902</v>
+      </c>
+      <c r="B45" s="2">
+        <v>3.3394827424560902E-2</v>
+      </c>
+      <c r="C45" s="2">
+        <v>0.52365074324704297</v>
+      </c>
+      <c r="D45" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52471450847284251</v>
+      </c>
+      <c r="E45" s="2">
+        <f t="shared" si="1"/>
+        <v>3.6489875956201647</v>
+      </c>
+      <c r="G45" s="12">
+        <v>0.4</v>
+      </c>
+      <c r="H45" s="13">
+        <v>0.36957282287551901</v>
+      </c>
+      <c r="I45" s="13">
+        <v>0.36904907307660501</v>
+      </c>
+      <c r="J45" s="14">
+        <f t="shared" si="2"/>
+        <v>0.52228468266538419</v>
+      </c>
+      <c r="K45" s="13">
+        <f t="shared" si="3"/>
+        <v>45.040627888414242</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A46" s="8">
+        <v>0.40999999999999898</v>
+      </c>
+      <c r="B46" s="2">
+        <v>3.4856268003829703E-2</v>
+      </c>
+      <c r="C46" s="2">
+        <v>0.52380351635492595</v>
+      </c>
+      <c r="D46" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52496198259011095</v>
+      </c>
+      <c r="E46" s="2">
+        <f t="shared" si="1"/>
+        <v>3.807108827974222</v>
+      </c>
+      <c r="G46" s="1">
+        <v>0.41</v>
+      </c>
+      <c r="H46" s="2">
+        <v>0.379000373676328</v>
+      </c>
+      <c r="I46" s="2">
+        <v>0.359872112050452</v>
+      </c>
+      <c r="J46" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52263679575633526</v>
+      </c>
+      <c r="K46" s="2">
+        <f t="shared" si="3"/>
+        <v>46.482967543767941</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A47" s="8">
+        <v>0.41999999999999899</v>
+      </c>
+      <c r="B47" s="2">
+        <v>3.6325271985735298E-2</v>
+      </c>
+      <c r="C47" s="2">
+        <v>0.52369181736645598</v>
+      </c>
+      <c r="D47" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52495013569044746</v>
+      </c>
+      <c r="E47" s="2">
+        <f t="shared" si="1"/>
+        <v>3.9678994107290193</v>
+      </c>
+      <c r="G47" s="1">
+        <v>0.42</v>
+      </c>
+      <c r="H47" s="2">
+        <v>0.38644404454592901</v>
+      </c>
+      <c r="I47" s="2">
+        <v>0.34738484430725602</v>
+      </c>
+      <c r="J47" s="4">
+        <f t="shared" si="2"/>
+        <v>0.5196298967721088</v>
+      </c>
+      <c r="K47" s="2">
+        <f t="shared" si="3"/>
+        <v>48.046783171765576</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A48" s="8">
+        <v>0.43</v>
+      </c>
+      <c r="B48" s="2">
+        <v>3.7870405620076798E-2</v>
+      </c>
+      <c r="C48" s="2">
+        <v>0.52380887083023098</v>
+      </c>
+      <c r="D48" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52517606645987858</v>
+      </c>
+      <c r="E48" s="2">
+        <f t="shared" si="1"/>
+        <v>4.1351832485646982</v>
+      </c>
+      <c r="G48" s="1">
+        <v>0.43</v>
+      </c>
+      <c r="H48" s="2">
+        <v>0.39425397693888697</v>
+      </c>
+      <c r="I48" s="2">
+        <v>0.33917004638377102</v>
+      </c>
+      <c r="J48" s="4">
+        <f t="shared" si="2"/>
+        <v>0.52006972484090808</v>
+      </c>
+      <c r="K48" s="2">
+        <f t="shared" si="3"/>
+        <v>49.295144954034456</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A49" s="8">
+        <v>0.44</v>
+      </c>
+      <c r="B49" s="2">
+        <v>3.9376000659696202E-2</v>
+      </c>
+      <c r="C49" s="2">
+        <v>0.52363284064321702</v>
+      </c>
+      <c r="D49" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52511124652595009</v>
+      </c>
+      <c r="E49" s="2">
+        <f t="shared" si="1"/>
+        <v>4.3004188535810934</v>
+      </c>
+      <c r="G49" s="12">
+        <v>0.44</v>
+      </c>
+      <c r="H49" s="13">
+        <v>0.40453656679911998</v>
+      </c>
+      <c r="I49" s="13">
+        <v>0.32637224896384898</v>
+      </c>
+      <c r="J49" s="14">
+        <f t="shared" si="2"/>
+        <v>0.51977752815155398</v>
+      </c>
+      <c r="K49" s="13">
+        <f t="shared" si="3"/>
+        <v>51.10408437945987</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A50" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="B50" s="2">
+        <v>4.0984334448909802E-2</v>
+      </c>
+      <c r="C50" s="2">
+        <v>0.52384588270690002</v>
+      </c>
+      <c r="D50" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52544669044460768</v>
+      </c>
+      <c r="E50" s="2">
+        <f t="shared" si="1"/>
+        <v>4.4735593940085607</v>
+      </c>
+      <c r="G50" s="12">
+        <v>0.45</v>
+      </c>
+      <c r="H50" s="13">
+        <v>0.41357190881515798</v>
+      </c>
+      <c r="I50" s="13">
+        <v>0.31470363992882899</v>
+      </c>
+      <c r="J50" s="14">
+        <f t="shared" si="2"/>
+        <v>0.51969231738160937</v>
+      </c>
+      <c r="K50" s="13">
+        <f t="shared" si="3"/>
+        <v>52.731021932633332</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A51" s="8">
+        <v>0.46</v>
+      </c>
+      <c r="B51" s="2">
+        <v>4.2728382603661998E-2</v>
+      </c>
+      <c r="C51" s="2">
+        <v>0.52357721669410495</v>
+      </c>
+      <c r="D51" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52531782429408458</v>
+      </c>
+      <c r="E51" s="2">
+        <f t="shared" si="1"/>
+        <v>4.6654870653573148</v>
+      </c>
+      <c r="G51" s="12">
+        <v>0.46</v>
+      </c>
+      <c r="H51" s="13">
+        <v>0.42477805005376201</v>
+      </c>
+      <c r="I51" s="13">
+        <v>0.300287789238664</v>
+      </c>
+      <c r="J51" s="14">
+        <f t="shared" si="2"/>
+        <v>0.52020106514050946</v>
+      </c>
+      <c r="K51" s="13">
+        <f t="shared" si="3"/>
+        <v>54.74241358091426</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A52" s="8">
+        <v>0.47</v>
+      </c>
+      <c r="B52" s="2">
+        <v>4.4364458431318997E-2</v>
+      </c>
+      <c r="C52" s="2">
+        <v>0.52368999609671596</v>
+      </c>
+      <c r="D52" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52556580671090336</v>
+      </c>
+      <c r="E52" s="2">
+        <f t="shared" si="1"/>
+        <v>4.8422569277079521</v>
+      </c>
+      <c r="G52" s="1">
+        <v>0.47</v>
+      </c>
+      <c r="H52" s="2">
+        <v>0.43254599096520702</v>
+      </c>
+      <c r="I52" s="2">
+        <v>0.28677268001183298</v>
+      </c>
+      <c r="J52" s="4">
+        <f t="shared" si="2"/>
+        <v>0.51897456999475622</v>
+      </c>
+      <c r="K52" s="2">
+        <f t="shared" si="3"/>
+        <v>56.45611062980953</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A53" s="8">
+        <v>0.48</v>
+      </c>
+      <c r="B53" s="2">
+        <v>4.63846027193687E-2</v>
+      </c>
+      <c r="C53" s="2">
+        <v>0.52371520716945097</v>
+      </c>
+      <c r="D53" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52576529895950219</v>
+      </c>
+      <c r="E53" s="2">
+        <f t="shared" si="1"/>
+        <v>5.0613869814528512</v>
+      </c>
+      <c r="G53" s="1">
+        <v>0.48</v>
+      </c>
+      <c r="H53" s="2">
+        <v>0.43944703209819802</v>
+      </c>
+      <c r="I53" s="2">
+        <v>0.27541934324568601</v>
+      </c>
+      <c r="J53" s="4">
+        <f t="shared" si="2"/>
+        <v>0.51862270356570361</v>
+      </c>
+      <c r="K53" s="2">
+        <f t="shared" si="3"/>
+        <v>57.922953257658079</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A54" s="8">
+        <v>0.49</v>
+      </c>
+      <c r="B54" s="2">
+        <v>4.8180493176457603E-2</v>
+      </c>
+      <c r="C54" s="2">
+        <v>0.52365978554513803</v>
+      </c>
+      <c r="D54" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52587159166464459</v>
+      </c>
+      <c r="E54" s="2">
+        <f t="shared" si="1"/>
+        <v>5.2568264556557995</v>
+      </c>
+      <c r="G54" s="6">
+        <v>0.49</v>
+      </c>
+      <c r="H54" s="5">
+        <v>0.44700548056450501</v>
+      </c>
+      <c r="I54" s="5">
+        <v>0.25977640230410098</v>
+      </c>
+      <c r="J54" s="7">
+        <f t="shared" si="2"/>
+        <v>0.51700839340262761</v>
+      </c>
+      <c r="K54" s="5">
+        <f t="shared" si="3"/>
+        <v>59.83706703540058</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A55" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="B55" s="2">
+        <v>4.9983915178053E-2</v>
+      </c>
+      <c r="C55" s="2">
+        <v>0.52369746306146303</v>
+      </c>
+      <c r="D55" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52607739410997234</v>
+      </c>
+      <c r="E55" s="2">
+        <f t="shared" si="1"/>
+        <v>5.4520378165490175</v>
+      </c>
+      <c r="G55" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="H55" s="13">
+        <v>0.45516609236207001</v>
+      </c>
+      <c r="I55" s="13">
+        <v>0.24661695930301</v>
+      </c>
+      <c r="J55" s="14">
+        <f t="shared" si="2"/>
+        <v>0.51768339383451245</v>
+      </c>
+      <c r="K55" s="13">
+        <f t="shared" si="3"/>
+        <v>61.550389618151385</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A56" s="8">
+        <v>0.51</v>
+      </c>
+      <c r="B56" s="2">
+        <v>5.2151733697974101E-2</v>
+      </c>
+      <c r="C56" s="2">
+        <v>0.52360278263448801</v>
+      </c>
+      <c r="D56" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52619357399181843</v>
+      </c>
+      <c r="E56" s="2">
+        <f t="shared" si="1"/>
+        <v>5.6879979841259685</v>
+      </c>
+      <c r="G56" s="1">
+        <v>0.51</v>
+      </c>
+      <c r="H56" s="2">
+        <v>0.46601826740700097</v>
+      </c>
+      <c r="I56" s="2">
+        <v>0.22740886273288299</v>
+      </c>
+      <c r="J56" s="14">
+        <f t="shared" si="2"/>
+        <v>0.51854393874240423</v>
+      </c>
+      <c r="K56" s="13">
+        <f t="shared" si="3"/>
+        <v>63.988423631939803</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A57" s="8">
+        <v>0.52</v>
+      </c>
+      <c r="B57" s="2">
+        <v>5.4094680841337998E-2</v>
+      </c>
+      <c r="C57" s="2">
+        <v>0.52373065076882697</v>
+      </c>
+      <c r="D57" s="2">
+        <f t="shared" si="0"/>
+        <v>0.5265168839173775</v>
+      </c>
+      <c r="E57" s="2">
+        <f t="shared" si="1"/>
+        <v>5.8970106206245987</v>
+      </c>
+      <c r="G57" s="1">
+        <v>0.52</v>
+      </c>
+      <c r="H57" s="2">
+        <v>0.47453784632518098</v>
+      </c>
+      <c r="I57" s="2">
+        <v>0.20909995136107801</v>
+      </c>
+      <c r="J57" s="14">
+        <f t="shared" si="2"/>
+        <v>0.51856432315976608</v>
+      </c>
+      <c r="K57" s="13">
+        <f t="shared" si="3"/>
+        <v>66.219832132379125</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A58" s="8">
+        <v>0.53</v>
+      </c>
+      <c r="B58" s="2">
+        <v>5.6131000753591502E-2</v>
+      </c>
+      <c r="C58" s="2">
+        <v>0.52354248577620899</v>
+      </c>
+      <c r="D58" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52654289821279676</v>
+      </c>
+      <c r="E58" s="2">
+        <f t="shared" si="1"/>
+        <v>6.1195244450719573</v>
+      </c>
+      <c r="G58" s="1">
+        <v>0.53</v>
+      </c>
+      <c r="H58" s="2">
+        <v>0.48307076449429198</v>
+      </c>
+      <c r="I58" s="2">
+        <v>0.19031337878329199</v>
+      </c>
+      <c r="J58" s="14">
+        <f t="shared" si="2"/>
+        <v>0.51920761324638964</v>
+      </c>
+      <c r="K58" s="13">
+        <f t="shared" si="3"/>
+        <v>68.497254073797066</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A59" s="8">
+        <v>0.53999999999999904</v>
+      </c>
+      <c r="B59" s="2">
+        <v>5.8470033123014298E-2</v>
+      </c>
+      <c r="C59" s="2">
+        <v>0.52364056174418905</v>
+      </c>
+      <c r="D59" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52689484973491274</v>
+      </c>
+      <c r="E59" s="2">
+        <f t="shared" si="1"/>
+        <v>6.3712908106833259</v>
+      </c>
+      <c r="G59" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="H59" s="2">
+        <v>0.49196780171281801</v>
+      </c>
+      <c r="I59" s="2">
+        <v>0.17057806191225</v>
+      </c>
+      <c r="J59" s="14">
+        <f t="shared" si="2"/>
+        <v>0.52070067517517393</v>
+      </c>
+      <c r="K59" s="13">
+        <f t="shared" si="3"/>
+        <v>70.877235371467179</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A60" s="8">
+        <v>0.54999999999999905</v>
+      </c>
+      <c r="B60" s="2">
+        <v>6.0848421767858499E-2</v>
+      </c>
+      <c r="C60" s="2">
+        <v>0.52340806880828294</v>
+      </c>
+      <c r="D60" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52693314274702385</v>
+      </c>
+      <c r="E60" s="2">
+        <f t="shared" si="1"/>
+        <v>6.6311125170463852</v>
+      </c>
+      <c r="G60" s="8">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H60" s="2">
+        <v>0.50085322073196104</v>
+      </c>
+      <c r="I60" s="2">
+        <v>0.14910673884560999</v>
+      </c>
+      <c r="J60" s="14">
+        <f t="shared" si="2"/>
+        <v>0.52257704531174298</v>
+      </c>
+      <c r="K60" s="13">
+        <f t="shared" si="3"/>
+        <v>73.421444112627995</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A61" s="8">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="B61" s="2">
+        <v>6.3553046240563599E-2</v>
+      </c>
+      <c r="C61" s="2">
+        <v>0.52342608112329003</v>
+      </c>
+      <c r="D61" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52727018888473132</v>
+      </c>
+      <c r="E61" s="2">
+        <f t="shared" si="1"/>
+        <v>6.9228194742617895</v>
+      </c>
+      <c r="G61" s="8">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="H61" s="2">
+        <v>0.51013541386809802</v>
+      </c>
+      <c r="I61" s="2">
+        <v>0.12707045787934201</v>
+      </c>
+      <c r="J61" s="14">
+        <f t="shared" si="2"/>
+        <v>0.52572335096326217</v>
+      </c>
+      <c r="K61" s="13">
+        <f t="shared" si="3"/>
+        <v>76.012751654003353</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A62" s="8">
+        <v>0.56999999999999895</v>
+      </c>
+      <c r="B62" s="2">
+        <v>6.6091718246011205E-2</v>
+      </c>
+      <c r="C62" s="2">
+        <v>0.52317499825113201</v>
+      </c>
+      <c r="D62" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52733309588511712</v>
+      </c>
+      <c r="E62" s="2">
+        <f t="shared" si="1"/>
+        <v>7.1999294909767011</v>
+      </c>
+      <c r="G62" s="1">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="H62" s="2">
+        <v>0.52069017111461602</v>
+      </c>
+      <c r="I62" s="2">
+        <v>0.10770279863325399</v>
+      </c>
+      <c r="J62" s="14">
+        <f t="shared" si="2"/>
+        <v>0.53171246659148719</v>
+      </c>
+      <c r="K62" s="13">
+        <f t="shared" si="3"/>
+        <v>78.313395748510032</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A63" s="8">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="B63" s="2">
+        <v>6.8737561689256793E-2</v>
+      </c>
+      <c r="C63" s="2">
+        <v>0.52333671038507901</v>
+      </c>
+      <c r="D63" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52783156861224245</v>
+      </c>
+      <c r="E63" s="2">
+        <f t="shared" si="1"/>
+        <v>7.4826705571693655</v>
+      </c>
+      <c r="G63" s="1">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="H63" s="2">
+        <v>0.52851489833389498</v>
+      </c>
+      <c r="I63" s="2">
+        <v>8.5145347314984507E-2</v>
+      </c>
+      <c r="J63" s="14">
+        <f t="shared" si="2"/>
+        <v>0.53532955077249067</v>
+      </c>
+      <c r="K63" s="13">
+        <f t="shared" si="3"/>
+        <v>80.848112694962907</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A64" s="8">
+        <v>0.58999999999999897</v>
+      </c>
+      <c r="B64" s="2">
+        <v>7.1796983486834096E-2</v>
+      </c>
+      <c r="C64" s="2">
+        <v>0.52324285090738198</v>
+      </c>
+      <c r="D64" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52814570703878061</v>
+      </c>
+      <c r="E64" s="2">
+        <f t="shared" si="1"/>
+        <v>7.8130727770476289</v>
+      </c>
+      <c r="G64" s="1">
+        <v>0.59</v>
+      </c>
+      <c r="H64" s="2">
+        <v>0.53799381958683101</v>
+      </c>
+      <c r="I64" s="2">
+        <v>5.6662602488040302E-2</v>
+      </c>
+      <c r="J64" s="14">
+        <f t="shared" si="2"/>
+        <v>0.54096950046591852</v>
+      </c>
+      <c r="K64" s="13">
+        <f t="shared" si="3"/>
+        <v>83.98765777052526</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A65" s="8">
+        <v>0.6</v>
+      </c>
+      <c r="B65" s="2">
+        <v>7.4911158113282403E-2</v>
+      </c>
+      <c r="C65" s="2">
+        <v>0.52309115566358499</v>
+      </c>
+      <c r="D65" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52842789360833142</v>
+      </c>
+      <c r="E65" s="2">
+        <f t="shared" si="1"/>
+        <v>8.1498363012683477</v>
+      </c>
+      <c r="G65" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="H65" s="2">
+        <v>0.54807205225288502</v>
+      </c>
+      <c r="I65" s="2">
+        <v>2.5161816152906101E-2</v>
+      </c>
+      <c r="J65" s="14">
+        <f t="shared" si="2"/>
+        <v>0.54864933377595726</v>
+      </c>
+      <c r="K65" s="13">
+        <f t="shared" si="3"/>
+        <v>87.37141443825</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A66" s="8">
+        <v>0.60999999999999899</v>
+      </c>
+      <c r="B66" s="2">
+        <v>7.7731801696820799E-2</v>
+      </c>
+      <c r="C66" s="2">
+        <v>0.52297142718388001</v>
+      </c>
+      <c r="D66" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52871669790709108</v>
+      </c>
+      <c r="E66" s="2">
+        <f t="shared" si="1"/>
+        <v>8.4542565280924862</v>
+      </c>
+      <c r="G66" s="1"/>
+      <c r="J66" s="14"/>
+      <c r="K66" s="13"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A67" s="8">
+        <v>0.62</v>
+      </c>
+      <c r="B67" s="2">
+        <v>8.1309516102914495E-2</v>
+      </c>
+      <c r="C67" s="2">
+        <v>0.52278402533770296</v>
+      </c>
+      <c r="D67" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52906934758799073</v>
+      </c>
+      <c r="E67" s="2">
+        <f t="shared" si="1"/>
+        <v>8.8404830115860502</v>
+      </c>
+      <c r="G67" s="1"/>
+      <c r="J67" s="14"/>
+      <c r="K67" s="13"/>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A68" s="8">
+        <v>0.62999999999999901</v>
+      </c>
+      <c r="B68" s="2">
+        <v>8.47065070154428E-2</v>
+      </c>
+      <c r="C68" s="2">
+        <v>0.52240827206249596</v>
+      </c>
+      <c r="D68" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52923113575268799</v>
+      </c>
+      <c r="E68" s="2">
+        <f t="shared" si="1"/>
+        <v>9.2101344301055796</v>
+      </c>
+      <c r="G68" s="1"/>
+      <c r="J68" s="3"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A69" s="8">
+        <v>0.64</v>
+      </c>
+      <c r="B69" s="2">
+        <v>8.8262232125514595E-2</v>
+      </c>
+      <c r="C69" s="2">
+        <v>0.52182699821709</v>
+      </c>
+      <c r="D69" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52923873411536793</v>
+      </c>
+      <c r="E69" s="2">
+        <f t="shared" si="1"/>
+        <v>9.6001923364142225</v>
+      </c>
+      <c r="G69" s="1"/>
+      <c r="J69" s="3"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A70" s="8">
+        <v>0.64999999999999902</v>
+      </c>
+      <c r="B70" s="2">
+        <v>9.1932308947797095E-2</v>
+      </c>
+      <c r="C70" s="2">
+        <v>0.52117651451233604</v>
+      </c>
+      <c r="D70" s="2">
+        <f t="shared" ref="D70:D131" si="7">(B70^2+C70^2)^0.5</f>
+        <v>0.52922255120856332</v>
+      </c>
+      <c r="E70" s="2">
+        <f t="shared" ref="E70:E131" si="8">DEGREES(ATAN(B70/C70))</f>
+        <v>10.003713307284933</v>
+      </c>
+      <c r="G70" s="1"/>
+      <c r="J70" s="3"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A71" s="8">
+        <v>0.66</v>
+      </c>
+      <c r="B71" s="2">
+        <v>9.5501670330632796E-2</v>
+      </c>
+      <c r="C71" s="2">
+        <v>0.52053948956017204</v>
+      </c>
+      <c r="D71" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52922767239393798</v>
+      </c>
+      <c r="E71" s="2">
+        <f t="shared" si="8"/>
+        <v>10.396251353050024</v>
+      </c>
+      <c r="G71" s="1"/>
+      <c r="J71" s="3"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A72" s="8">
+        <v>0.66999999999999904</v>
+      </c>
+      <c r="B72" s="2">
+        <v>9.9453482525175302E-2</v>
+      </c>
+      <c r="C72" s="2">
+        <v>0.51966744477290405</v>
+      </c>
+      <c r="D72" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52909852423077564</v>
+      </c>
+      <c r="E72" s="2">
+        <f t="shared" si="8"/>
+        <v>10.834210689021106</v>
+      </c>
+      <c r="G72" s="1"/>
+      <c r="J72" s="3"/>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A73" s="8">
+        <v>0.67999999999999905</v>
+      </c>
+      <c r="B73" s="2">
+        <v>0.103126645350799</v>
+      </c>
+      <c r="C73" s="2">
+        <v>0.51885022684974402</v>
+      </c>
+      <c r="D73" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52899968136411979</v>
+      </c>
+      <c r="E73" s="2">
+        <f t="shared" si="8"/>
+        <v>11.241599279396224</v>
+      </c>
+      <c r="G73" s="1"/>
+      <c r="J73" s="3"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A74" s="8">
+        <v>0.68999999999999895</v>
+      </c>
+      <c r="B74" s="2">
+        <v>0.10716608097091999</v>
+      </c>
+      <c r="C74" s="2">
+        <v>0.51820088931388797</v>
+      </c>
+      <c r="D74" s="2">
+        <f t="shared" si="7"/>
+        <v>0.5291660709043714</v>
+      </c>
+      <c r="E74" s="2">
+        <f t="shared" si="8"/>
+        <v>11.684290747969166</v>
+      </c>
+      <c r="G74" s="1"/>
+      <c r="J74" s="3"/>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A75" s="8">
+        <v>0.69999999999999896</v>
+      </c>
+      <c r="B75" s="2">
+        <v>0.11266748084415799</v>
+      </c>
+      <c r="C75" s="2">
+        <v>0.51556017577714797</v>
+      </c>
+      <c r="D75" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52772744488716183</v>
+      </c>
+      <c r="E75" s="2">
+        <f t="shared" si="8"/>
+        <v>12.327281682287392</v>
+      </c>
+      <c r="G75" s="1"/>
+      <c r="J75" s="3"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A76" s="8">
+        <v>0.70999999999999897</v>
+      </c>
+      <c r="B76" s="2">
+        <v>0.116691331598282</v>
+      </c>
+      <c r="C76" s="2">
+        <v>0.51472978929435498</v>
+      </c>
+      <c r="D76" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52779126826539224</v>
+      </c>
+      <c r="E76" s="2">
+        <f t="shared" si="8"/>
+        <v>12.773280179661976</v>
+      </c>
+      <c r="G76" s="1"/>
+      <c r="J76" s="3"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A77" s="8">
+        <v>0.71999999999999897</v>
+      </c>
+      <c r="B77" s="2">
+        <v>0.123309988154952</v>
+      </c>
+      <c r="C77" s="2">
+        <v>0.51222714968053396</v>
+      </c>
+      <c r="D77" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52686051858971039</v>
+      </c>
+      <c r="E77" s="2">
+        <f t="shared" si="8"/>
+        <v>13.535438181566718</v>
+      </c>
+      <c r="G77" s="1"/>
+      <c r="J77" s="3"/>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A78" s="8">
+        <v>0.72999999999999898</v>
+      </c>
+      <c r="B78" s="2">
+        <v>0.12790614061318001</v>
+      </c>
+      <c r="C78" s="2">
+        <v>0.510087631034848</v>
+      </c>
+      <c r="D78" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52587961753741874</v>
+      </c>
+      <c r="E78" s="2">
+        <f t="shared" si="8"/>
+        <v>14.076856588286393</v>
+      </c>
+      <c r="G78" s="1"/>
+      <c r="J78" s="3"/>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A79" s="8">
+        <v>0.73999999999999899</v>
+      </c>
+      <c r="B79" s="2">
+        <v>0.13187011260991699</v>
+      </c>
+      <c r="C79" s="2">
+        <v>0.50760906776930703</v>
+      </c>
+      <c r="D79" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52445847526889788</v>
+      </c>
+      <c r="E79" s="2">
+        <f t="shared" si="8"/>
+        <v>14.562771215615857</v>
+      </c>
+      <c r="G79" s="1"/>
+      <c r="J79" s="3"/>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A80" s="8">
+        <v>0.749999999999999</v>
+      </c>
+      <c r="B80" s="2">
+        <v>0.13599361185967901</v>
+      </c>
+      <c r="C80" s="2">
+        <v>0.50512066495672903</v>
+      </c>
+      <c r="D80" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52310720567869173</v>
+      </c>
+      <c r="E80" s="2">
+        <f t="shared" si="8"/>
+        <v>15.068444445172528</v>
+      </c>
+      <c r="G80" s="1"/>
+      <c r="J80" s="3"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A81" s="8">
+        <v>0.75999999999999901</v>
+      </c>
+      <c r="B81" s="2">
+        <v>0.13998888818741201</v>
+      </c>
+      <c r="C81" s="2">
+        <v>0.50288745337793195</v>
+      </c>
+      <c r="D81" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52200831370859357</v>
+      </c>
+      <c r="E81" s="2">
+        <f t="shared" si="8"/>
+        <v>15.555618767891753</v>
+      </c>
+      <c r="G81" s="1"/>
+      <c r="J81" s="3"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A82" s="8">
+        <v>0.76999999999999902</v>
+      </c>
+      <c r="B82" s="2">
+        <v>0.14401649199057601</v>
+      </c>
+      <c r="C82" s="2">
+        <v>0.50084351111964198</v>
+      </c>
+      <c r="D82" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52113815116140039</v>
+      </c>
+      <c r="E82" s="2">
+        <f t="shared" si="8"/>
+        <v>16.042477382512594</v>
+      </c>
+      <c r="G82" s="1"/>
+      <c r="J82" s="3"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A83" s="8">
+        <v>0.77999999999999903</v>
+      </c>
+      <c r="B83" s="2">
+        <v>0.14797505909452</v>
+      </c>
+      <c r="C83" s="2">
+        <v>0.49890489088418499</v>
+      </c>
+      <c r="D83" s="2">
+        <f t="shared" si="7"/>
+        <v>0.5203870754180846</v>
+      </c>
+      <c r="E83" s="2">
+        <f t="shared" si="8"/>
+        <v>16.520342750019456</v>
+      </c>
+      <c r="G83" s="1"/>
+      <c r="J83" s="3"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A84" s="8">
+        <v>0.78999999999999904</v>
+      </c>
+      <c r="B84" s="2">
+        <v>0.15236859077954801</v>
+      </c>
+      <c r="C84" s="2">
+        <v>0.49700761450289299</v>
+      </c>
+      <c r="D84" s="2">
+        <f t="shared" si="7"/>
+        <v>0.51983916390553109</v>
+      </c>
+      <c r="E84" s="2">
+        <f t="shared" si="8"/>
+        <v>17.04407017920941</v>
+      </c>
+      <c r="G84" s="1"/>
+      <c r="J84" s="3"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A85" s="8">
+        <v>0.79999999999999905</v>
+      </c>
+      <c r="B85" s="2">
+        <v>0.15663341479384399</v>
+      </c>
+      <c r="C85" s="2">
+        <v>0.49494438176116201</v>
+      </c>
+      <c r="D85" s="2">
+        <f t="shared" si="7"/>
+        <v>0.51913771551190468</v>
+      </c>
+      <c r="E85" s="2">
+        <f t="shared" si="8"/>
+        <v>17.560845089871584</v>
+      </c>
+      <c r="G85" s="1"/>
+      <c r="J85" s="3"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A86" s="8">
+        <v>0.81</v>
+      </c>
+      <c r="B86" s="2">
+        <v>0.161382660237716</v>
+      </c>
+      <c r="C86" s="2">
+        <v>0.49294402795618703</v>
+      </c>
+      <c r="D86" s="2">
+        <f t="shared" si="7"/>
+        <v>0.51868890264114209</v>
+      </c>
+      <c r="E86" s="2">
+        <f t="shared" si="8"/>
+        <v>18.127689328984669</v>
+      </c>
+      <c r="G86" s="1"/>
+      <c r="J86" s="3"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A87" s="8">
+        <v>0.81999999999999895</v>
+      </c>
+      <c r="B87" s="2">
+        <v>0.16500900596628401</v>
+      </c>
+      <c r="C87" s="2">
+        <v>0.49120789968848499</v>
+      </c>
+      <c r="D87" s="2">
+        <f t="shared" si="7"/>
+        <v>0.51818256702281473</v>
+      </c>
+      <c r="E87" s="2">
+        <f t="shared" si="8"/>
+        <v>18.568486349686317</v>
+      </c>
+      <c r="G87" s="1"/>
+      <c r="J87" s="3"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A88" s="8">
+        <v>0.83</v>
+      </c>
+      <c r="B88" s="2">
+        <v>0.16984095490335999</v>
+      </c>
+      <c r="C88" s="2">
+        <v>0.48937267916977401</v>
+      </c>
+      <c r="D88" s="2">
+        <f t="shared" si="7"/>
+        <v>0.5180073060105308</v>
+      </c>
+      <c r="E88" s="2">
+        <f t="shared" si="8"/>
+        <v>19.139766438632034</v>
+      </c>
+      <c r="G88" s="1"/>
+      <c r="J88" s="3"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A89" s="8">
+        <v>0.83999999999999897</v>
+      </c>
+      <c r="B89" s="2">
+        <v>0.17497274626257001</v>
+      </c>
+      <c r="C89" s="2">
+        <v>0.487668212079305</v>
+      </c>
+      <c r="D89" s="2">
+        <f t="shared" si="7"/>
+        <v>0.51810785267865966</v>
+      </c>
+      <c r="E89" s="2">
+        <f t="shared" si="8"/>
+        <v>19.737714980713669</v>
+      </c>
+      <c r="G89" s="1"/>
+      <c r="J89" s="3"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A90" s="8">
+        <v>0.85</v>
+      </c>
+      <c r="B90" s="2">
+        <v>0.17992976131185201</v>
+      </c>
+      <c r="C90" s="2">
+        <v>0.48605620133204802</v>
+      </c>
+      <c r="D90" s="2">
+        <f t="shared" si="7"/>
+        <v>0.5182907966181538</v>
+      </c>
+      <c r="E90" s="2">
+        <f t="shared" si="8"/>
+        <v>20.313697641408567</v>
+      </c>
+      <c r="G90" s="1"/>
+      <c r="J90" s="3"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A91" s="8">
+        <v>0.85999999999999899</v>
+      </c>
+      <c r="B91" s="2">
+        <v>0.18548072576463501</v>
+      </c>
+      <c r="C91" s="2">
+        <v>0.48437871943974198</v>
+      </c>
+      <c r="D91" s="2">
+        <f t="shared" si="7"/>
+        <v>0.51867701267384114</v>
+      </c>
+      <c r="E91" s="2">
+        <f t="shared" si="8"/>
+        <v>20.953092762777612</v>
+      </c>
+      <c r="G91" s="1"/>
+      <c r="J91" s="3"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A92" s="8">
+        <v>0.87</v>
+      </c>
+      <c r="B92" s="2">
+        <v>0.191698777788018</v>
+      </c>
+      <c r="C92" s="2">
+        <v>0.48249285066893199</v>
+      </c>
+      <c r="D92" s="2">
+        <f t="shared" si="7"/>
+        <v>0.51917990364810174</v>
+      </c>
+      <c r="E92" s="2">
+        <f t="shared" si="8"/>
+        <v>21.668372587979302</v>
+      </c>
+      <c r="G92" s="1"/>
+      <c r="J92" s="3"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A93" s="8">
+        <v>0.87999999999999901</v>
+      </c>
+      <c r="B93" s="2">
+        <v>0.19830937267203599</v>
+      </c>
+      <c r="C93" s="2">
+        <v>0.48050429409652601</v>
+      </c>
+      <c r="D93" s="2">
+        <f t="shared" si="7"/>
+        <v>0.51981822201109618</v>
+      </c>
+      <c r="E93" s="2">
+        <f t="shared" si="8"/>
+        <v>22.426474588698113</v>
+      </c>
+      <c r="G93" s="1"/>
+      <c r="J93" s="3"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A94" s="8">
+        <v>0.89</v>
+      </c>
+      <c r="B94" s="2">
+        <v>0.20556331525944699</v>
+      </c>
+      <c r="C94" s="2">
+        <v>0.47898672404716403</v>
+      </c>
+      <c r="D94" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52123368885164056</v>
+      </c>
+      <c r="E94" s="2">
+        <f t="shared" si="8"/>
+        <v>23.227212942481518</v>
+      </c>
+      <c r="G94" s="1"/>
+      <c r="J94" s="3"/>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A95" s="8">
+        <v>0.89999999999999902</v>
+      </c>
+      <c r="B95" s="2">
+        <v>0.213149767069711</v>
+      </c>
+      <c r="C95" s="2">
+        <v>0.47673360184408697</v>
+      </c>
+      <c r="D95" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52221427625938044</v>
+      </c>
+      <c r="E95" s="2">
+        <f t="shared" si="8"/>
+        <v>24.089636256894188</v>
+      </c>
+      <c r="G95" s="1"/>
+      <c r="J95" s="3"/>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A96" s="8">
+        <v>0.91</v>
+      </c>
+      <c r="B96" s="2">
+        <v>0.221262809217633</v>
+      </c>
+      <c r="C96" s="2">
+        <v>0.47429174238925198</v>
+      </c>
+      <c r="D96" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52336401064795346</v>
+      </c>
+      <c r="E96" s="2">
+        <f t="shared" si="8"/>
+        <v>25.009618038112752</v>
+      </c>
+      <c r="G96" s="1"/>
+      <c r="J96" s="3"/>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A97" s="8">
+        <v>0.91999999999999904</v>
+      </c>
+      <c r="B97" s="2">
+        <v>0.22968440534311699</v>
+      </c>
+      <c r="C97" s="2">
+        <v>0.47123200321540698</v>
+      </c>
+      <c r="D97" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52422755260690623</v>
+      </c>
+      <c r="E97" s="2">
+        <f t="shared" si="8"/>
+        <v>25.985186332403728</v>
+      </c>
+      <c r="G97" s="1"/>
+      <c r="J97" s="3"/>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A98" s="8">
+        <v>0.92999999999999905</v>
+      </c>
+      <c r="B98" s="2">
+        <v>0.23841731413289699</v>
+      </c>
+      <c r="C98" s="2">
+        <v>0.46738031834958998</v>
+      </c>
+      <c r="D98" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52467816579204873</v>
+      </c>
+      <c r="E98" s="2">
+        <f t="shared" si="8"/>
+        <v>27.026771694518068</v>
+      </c>
+      <c r="G98" s="1"/>
+      <c r="J98" s="3"/>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A99" s="8">
+        <v>0.93999999999999895</v>
+      </c>
+      <c r="B99" s="2">
+        <v>0.24663715012352599</v>
+      </c>
+      <c r="C99" s="2">
+        <v>0.46351780228410999</v>
+      </c>
+      <c r="D99" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52505108023443392</v>
+      </c>
+      <c r="E99" s="2">
+        <f t="shared" si="8"/>
+        <v>28.017378137687079</v>
+      </c>
+      <c r="G99" s="1"/>
+      <c r="J99" s="3"/>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A100" s="8">
+        <v>0.94999999999999896</v>
+      </c>
+      <c r="B100" s="2">
+        <v>0.25478326955286801</v>
+      </c>
+      <c r="C100" s="2">
+        <v>0.458720980304477</v>
+      </c>
+      <c r="D100" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52472797925739556</v>
+      </c>
+      <c r="E100" s="2">
+        <f t="shared" si="8"/>
+        <v>29.048712944429404</v>
+      </c>
+      <c r="G100" s="1"/>
+      <c r="J100" s="3"/>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A101" s="8">
+        <v>0.95999999999999897</v>
+      </c>
+      <c r="B101" s="2">
+        <v>0.26433987886069299</v>
+      </c>
+      <c r="C101" s="2">
+        <v>0.45222473897698001</v>
+      </c>
+      <c r="D101" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52381560314569053</v>
+      </c>
+      <c r="E101" s="2">
+        <f t="shared" si="8"/>
+        <v>30.307656959062655</v>
+      </c>
+      <c r="G101" s="1"/>
+      <c r="J101" s="3"/>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A102" s="8">
+        <v>0.96999999999999897</v>
+      </c>
+      <c r="B102" s="2">
+        <v>0.27320421150163898</v>
+      </c>
+      <c r="C102" s="2">
+        <v>0.44479132337985799</v>
+      </c>
+      <c r="D102" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52199603689706087</v>
+      </c>
+      <c r="E102" s="2">
+        <f t="shared" si="8"/>
+        <v>31.559497599871911</v>
+      </c>
+      <c r="G102" s="1"/>
+      <c r="J102" s="3"/>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A103" s="8">
+        <v>0.97999999999999898</v>
+      </c>
+      <c r="B103" s="2">
+        <v>0.28176371451816401</v>
+      </c>
+      <c r="C103" s="2">
+        <v>0.437621003478806</v>
+      </c>
+      <c r="D103" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52048336525279126</v>
+      </c>
+      <c r="E103" s="2">
+        <f t="shared" si="8"/>
+        <v>32.775592419663361</v>
+      </c>
+      <c r="G103" s="1"/>
+      <c r="J103" s="3"/>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A104" s="8">
+        <v>0.98999999999999899</v>
+      </c>
+      <c r="B104" s="2">
+        <v>0.2892262562058</v>
+      </c>
+      <c r="C104" s="2">
+        <v>0.430066014970716</v>
+      </c>
+      <c r="D104" s="2">
+        <f t="shared" si="7"/>
+        <v>0.51827464197239592</v>
+      </c>
+      <c r="E104" s="2">
+        <f t="shared" si="8"/>
+        <v>33.921461203470301</v>
+      </c>
+      <c r="G104" s="1"/>
+      <c r="J104" s="3"/>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A105" s="8">
+        <v>0.999999999999999</v>
+      </c>
+      <c r="B105" s="2">
+        <v>0.29681647829381802</v>
+      </c>
+      <c r="C105" s="2">
+        <v>0.42736981117655798</v>
+      </c>
+      <c r="D105" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52033160320302607</v>
+      </c>
+      <c r="E105" s="2">
+        <f t="shared" si="8"/>
+        <v>34.780715382052485</v>
+      </c>
+      <c r="G105" s="1"/>
+      <c r="J105" s="3"/>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A106" s="8">
+        <v>1.00999999999999</v>
+      </c>
+      <c r="B106" s="2">
+        <v>0.30521584020338499</v>
+      </c>
+      <c r="C106" s="2">
+        <v>0.41998682693620898</v>
+      </c>
+      <c r="D106" s="2">
+        <f t="shared" si="7"/>
+        <v>0.51917785383335002</v>
+      </c>
+      <c r="E106" s="2">
+        <f t="shared" si="8"/>
+        <v>36.006923753880208</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A107" s="15">
+        <v>1.01999999999999</v>
+      </c>
+      <c r="B107" s="13">
+        <v>0.31354771743016702</v>
+      </c>
+      <c r="C107" s="13">
+        <v>0.41336655990654703</v>
+      </c>
+      <c r="D107" s="13">
+        <f t="shared" si="7"/>
+        <v>0.51882953265464826</v>
+      </c>
+      <c r="E107" s="13">
+        <f t="shared" si="8"/>
+        <v>37.181124989288762</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A108" s="15">
+        <v>1.02999999999999</v>
+      </c>
+      <c r="B108" s="13">
+        <v>0.32236202962362298</v>
+      </c>
+      <c r="C108" s="13">
+        <v>0.406012942555186</v>
+      </c>
+      <c r="D108" s="13">
+        <f t="shared" si="7"/>
+        <v>0.51842433166797097</v>
+      </c>
+      <c r="E108" s="13">
+        <f t="shared" si="8"/>
+        <v>38.448515170745232</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A109" s="8">
+        <v>1.03999999999999</v>
+      </c>
+      <c r="B109" s="2">
+        <v>0.33120429312085198</v>
+      </c>
+      <c r="C109" s="2">
+        <v>0.398696694585151</v>
+      </c>
+      <c r="D109" s="2">
+        <f t="shared" si="7"/>
+        <v>0.51831972570490548</v>
+      </c>
+      <c r="E109" s="2">
+        <f t="shared" si="8"/>
+        <v>39.717003288580294</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A110" s="8">
+        <v>1.0499999999999901</v>
+      </c>
+      <c r="B110" s="2">
+        <v>0.34041351241952</v>
+      </c>
+      <c r="C110" s="2">
+        <v>0.39101901082104001</v>
+      </c>
+      <c r="D110" s="2">
+        <f t="shared" si="7"/>
+        <v>0.51843729250629655</v>
+      </c>
+      <c r="E110" s="2">
+        <f t="shared" si="8"/>
+        <v>41.042193641661051</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A111" s="8">
+        <v>1.06</v>
+      </c>
+      <c r="B111" s="2">
+        <v>0.35092729711486298</v>
+      </c>
+      <c r="C111" s="2">
+        <v>0.38286096112717599</v>
+      </c>
+      <c r="D111" s="2">
+        <f t="shared" si="7"/>
+        <v>0.51935776052309868</v>
+      </c>
+      <c r="E111" s="2">
+        <f t="shared" si="8"/>
+        <v>42.508122543056444</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A112" s="15">
+        <v>1.0699999999999901</v>
+      </c>
+      <c r="B112" s="13">
+        <v>0.36240027326555702</v>
+      </c>
+      <c r="C112" s="13">
+        <v>0.37429449301634998</v>
+      </c>
+      <c r="D112" s="13">
+        <f t="shared" si="7"/>
+        <v>0.52098975572012629</v>
+      </c>
+      <c r="E112" s="13">
+        <f t="shared" si="8"/>
+        <v>44.075018016348558</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A113" s="8">
+        <v>1.08</v>
+      </c>
+      <c r="B113" s="2">
+        <v>0.37462003291301699</v>
+      </c>
+      <c r="C113" s="2">
+        <v>0.36422547161675101</v>
+      </c>
+      <c r="D113" s="2">
+        <f t="shared" si="7"/>
+        <v>0.5224943667009192</v>
+      </c>
+      <c r="E113" s="2">
+        <f t="shared" si="8"/>
+        <v>45.806021286472834</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A114" s="8">
+        <v>1.0899999999999901</v>
+      </c>
+      <c r="B114" s="2">
+        <v>0.38614486860284503</v>
+      </c>
+      <c r="C114" s="2">
+        <v>0.35216468401595902</v>
+      </c>
+      <c r="D114" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52261632601399732</v>
+      </c>
+      <c r="E114" s="2">
+        <f t="shared" si="8"/>
+        <v>47.635138908247946</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A115" s="8">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B115" s="2">
+        <v>0.39745221936360903</v>
+      </c>
+      <c r="C115" s="2">
+        <v>0.33954208382038698</v>
+      </c>
+      <c r="D115" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52273998638151753</v>
+      </c>
+      <c r="E115" s="2">
+        <f t="shared" si="8"/>
+        <v>49.492847295793666</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A116" s="10">
+        <v>1.1099999999999901</v>
+      </c>
+      <c r="B116" s="11">
+        <v>0.40649307700391102</v>
+      </c>
+      <c r="C116" s="11">
+        <v>0.32789032536930601</v>
+      </c>
+      <c r="D116" s="11">
+        <f t="shared" si="7"/>
+        <v>0.52225347018751045</v>
+      </c>
+      <c r="E116" s="2">
+        <f t="shared" si="8"/>
+        <v>51.109241466687152</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A117" s="8">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="B117" s="2">
+        <v>0.42187310516420801</v>
+      </c>
+      <c r="C117" s="2">
+        <v>0.30747939915993699</v>
+      </c>
+      <c r="D117" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52203495837792968</v>
+      </c>
+      <c r="E117" s="2">
+        <f t="shared" si="8"/>
+        <v>53.913812933834755</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A118" s="9">
+        <v>1.1299999999999899</v>
+      </c>
+      <c r="B118" s="5">
+        <v>0.43419470174130298</v>
+      </c>
+      <c r="C118" s="5">
+        <v>0.29215747477723902</v>
+      </c>
+      <c r="D118" s="5">
+        <f t="shared" si="7"/>
+        <v>0.52333643967187315</v>
+      </c>
+      <c r="E118" s="5">
+        <f t="shared" si="8"/>
+        <v>56.064492662935187</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A119" s="8">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="B119" s="2">
+        <v>0.44274073612540699</v>
+      </c>
+      <c r="C119" s="2">
+        <v>0.27690145307776098</v>
+      </c>
+      <c r="D119" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52220089442803785</v>
+      </c>
+      <c r="E119" s="2">
+        <f t="shared" si="8"/>
+        <v>57.977078986926031</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A120" s="8">
+        <v>1.1499999999999899</v>
+      </c>
+      <c r="B120" s="2">
+        <v>0.45377086062989602</v>
+      </c>
+      <c r="C120" s="2">
+        <v>0.25971371515964098</v>
+      </c>
+      <c r="D120" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52283764956133338</v>
+      </c>
+      <c r="E120" s="2">
+        <f t="shared" si="8"/>
+        <v>60.215529701188849</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A121" s="8">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="B121" s="2">
+        <v>0.46479000135384801</v>
+      </c>
+      <c r="C121" s="2">
+        <v>0.24189671687602199</v>
+      </c>
+      <c r="D121" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52396924241209841</v>
+      </c>
+      <c r="E121" s="2">
+        <f t="shared" si="8"/>
+        <v>62.505591061342621</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A122" s="8">
+        <v>1.1699999999999899</v>
+      </c>
+      <c r="B122" s="2">
+        <v>0.473921360981305</v>
+      </c>
+      <c r="C122" s="2">
+        <v>0.22411266993401299</v>
+      </c>
+      <c r="D122" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52424035062109087</v>
+      </c>
+      <c r="E122" s="2">
+        <f t="shared" si="8"/>
+        <v>64.691001494981975</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A123" s="15">
+        <v>1.18</v>
+      </c>
+      <c r="B123" s="13">
+        <v>0.48301976926715101</v>
+      </c>
+      <c r="C123" s="13">
+        <v>0.20444084189550699</v>
+      </c>
+      <c r="D123" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52450372290178793</v>
+      </c>
+      <c r="E123" s="2">
+        <f t="shared" si="8"/>
+        <v>67.059214949828871</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A124" s="8">
+        <v>1.18999999999999</v>
+      </c>
+      <c r="B124" s="2">
+        <v>0.49463521901499302</v>
+      </c>
+      <c r="C124" s="2">
+        <v>0.184725078734856</v>
+      </c>
+      <c r="D124" s="2">
+        <f t="shared" si="7"/>
+        <v>0.52800317669840668</v>
+      </c>
+      <c r="E124" s="2">
+        <f t="shared" si="8"/>
+        <v>69.521492388626967</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A125" s="8">
+        <v>1.19999999999999</v>
+      </c>
+      <c r="B125" s="2">
+        <v>0.50499214803183601</v>
+      </c>
+      <c r="C125" s="2">
+        <v>0.16503128313527801</v>
+      </c>
+      <c r="D125" s="2">
+        <f t="shared" si="7"/>
+        <v>0.53127431143156556</v>
+      </c>
+      <c r="E125" s="2">
+        <f t="shared" si="8"/>
+        <v>71.902623537137984</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A126" s="8">
+        <v>1.20999999999999</v>
+      </c>
+      <c r="B126" s="2">
+        <v>0.51466489778049895</v>
+      </c>
+      <c r="C126" s="2">
+        <v>0.14220216948874301</v>
+      </c>
+      <c r="D126" s="2">
+        <f t="shared" si="7"/>
+        <v>0.53394888708069865</v>
+      </c>
+      <c r="E126" s="2">
+        <f t="shared" si="8"/>
+        <v>74.55449742454023</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A127" s="8">
+        <v>1.21999999999999</v>
+      </c>
+      <c r="B127" s="2">
+        <v>0.52805829081947098</v>
+      </c>
+      <c r="C127" s="2">
+        <v>0.11616085133149601</v>
+      </c>
+      <c r="D127" s="2">
+        <f t="shared" si="7"/>
+        <v>0.54068373554716709</v>
+      </c>
+      <c r="E127" s="2">
+        <f t="shared" si="8"/>
+        <v>77.593820571761967</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A128" s="8">
+        <v>1.22999999999999</v>
+      </c>
+      <c r="B128" s="2">
+        <v>0.53649448739821004</v>
+      </c>
+      <c r="C128" s="2">
+        <v>9.4612225977032005E-2</v>
+      </c>
+      <c r="D128" s="2">
+        <f t="shared" si="7"/>
+        <v>0.54477317143284243</v>
+      </c>
+      <c r="E128" s="2">
+        <f t="shared" si="8"/>
+        <v>79.998573466041421</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A129" s="8">
+        <v>1.23999999999999</v>
+      </c>
+      <c r="B129" s="2">
+        <v>0.54910484714417096</v>
+      </c>
+      <c r="C129" s="2">
+        <v>5.9772246483341E-2</v>
+      </c>
+      <c r="D129" s="2">
+        <f t="shared" si="7"/>
+        <v>0.55234849018250121</v>
+      </c>
+      <c r="E129" s="2">
+        <f t="shared" si="8"/>
+        <v>83.787586822262298</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A130" s="8">
+        <v>1.24999999999999</v>
+      </c>
+      <c r="B130" s="2">
+        <v>0.55621662030869401</v>
+      </c>
+      <c r="C130" s="2">
+        <v>3.4470026496957802E-2</v>
+      </c>
+      <c r="D130" s="2">
+        <f t="shared" si="7"/>
+        <v>0.55728369026405833</v>
+      </c>
+      <c r="E130" s="2">
+        <f t="shared" si="8"/>
+        <v>86.453783616414455</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A131" s="8">
+        <v>1.25999999999999</v>
+      </c>
+      <c r="B131" s="2">
+        <v>0.56831854127505799</v>
+      </c>
+      <c r="C131" s="2">
+        <v>6.5628948042879501E-3</v>
+      </c>
+      <c r="D131" s="2">
+        <f t="shared" si="7"/>
+        <v>0.56835643389093604</v>
+      </c>
+      <c r="E131" s="2">
+        <f t="shared" si="8"/>
+        <v>89.338382556977365</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A132" s="8"/>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A133" s="8"/>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A134" s="8"/>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A135" s="8"/>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A136" s="8"/>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A137" s="8"/>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A138" s="8"/>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A139" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B58BE6-65FB-F14F-AB37-8104F299DF65}">
+  <dimension ref="A3:Q139"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="L18" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="11.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="2"/>
+    <col min="7" max="7" width="14.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.83203125" style="2"/>
+    <col min="13" max="13" width="16.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.83203125" style="2"/>
+    <col min="19" max="21" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M3" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" s="8">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2">
         <v>6.8033508512901899E-3</v>
       </c>
       <c r="C5" s="2">
@@ -20103,11 +24379,11 @@
         <v>0.50774966944220901</v>
       </c>
       <c r="D70" s="2">
-        <f t="shared" ref="D70:D120" si="7">(B70^2+C70^2)^0.5</f>
+        <f t="shared" ref="D70:D118" si="7">(B70^2+C70^2)^0.5</f>
         <v>0.52253441670288492</v>
       </c>
       <c r="E70" s="2">
-        <f t="shared" ref="E70:E120" si="8">DEGREES(ATAN(B70/C70))</f>
+        <f t="shared" ref="E70:E118" si="8">DEGREES(ATAN(B70/C70))</f>
         <v>13.662069522404304</v>
       </c>
       <c r="G70" s="1"/>

</xml_diff>